<commit_message>
Accessing Objects via dot notation, variables
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C9FC3F-41DE-46D2-81B4-6789EB2AA634}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6594343-D10D-46E3-8E27-1999FF3EB6CA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="346">
   <si>
     <t>Basic JavaScript</t>
   </si>
@@ -1061,6 +1061,21 @@
   </si>
   <si>
     <t>PassedReturning Boolean Values from Functions</t>
+  </si>
+  <si>
+    <t>PassedCounting Cards</t>
+  </si>
+  <si>
+    <t>PassedBuild JavaScript Objects</t>
+  </si>
+  <si>
+    <t>PassedAccessing Object Properties with Dot Notation</t>
+  </si>
+  <si>
+    <t>PassedAccessing Object Properties with Bracket Notation</t>
+  </si>
+  <si>
+    <t>PassedAccessing Object Properties with Variables</t>
   </si>
 </sst>
 </file>
@@ -7566,8 +7581,8 @@
   <dimension ref="A1:F299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E108" sqref="E108"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D81" sqref="D81:D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -8951,7 +8966,7 @@
         <v>80</v>
       </c>
       <c r="D81" t="s">
-        <v>80</v>
+        <v>341</v>
       </c>
       <c r="E81" s="2">
         <v>43432</v>
@@ -8968,7 +8983,7 @@
         <v>81</v>
       </c>
       <c r="D82" t="s">
-        <v>81</v>
+        <v>342</v>
       </c>
       <c r="E82" s="2">
         <v>43432</v>
@@ -8985,7 +9000,7 @@
         <v>82</v>
       </c>
       <c r="D83" t="s">
-        <v>82</v>
+        <v>343</v>
       </c>
       <c r="E83" s="2">
         <v>43432</v>
@@ -9002,7 +9017,7 @@
         <v>83</v>
       </c>
       <c r="D84" t="s">
-        <v>83</v>
+        <v>344</v>
       </c>
       <c r="E84" s="2">
         <v>43432</v>
@@ -9019,7 +9034,7 @@
         <v>84</v>
       </c>
       <c r="D85" t="s">
-        <v>84</v>
+        <v>345</v>
       </c>
       <c r="E85" s="2">
         <v>43432</v>

</xml_diff>

<commit_message>
Record collection - Review
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6594343-D10D-46E3-8E27-1999FF3EB6CA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB02C4A-A91C-4D4A-8DC1-3A7611BF6A24}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="355">
   <si>
     <t>Basic JavaScript</t>
   </si>
@@ -1076,6 +1076,33 @@
   </si>
   <si>
     <t>PassedAccessing Object Properties with Variables</t>
+  </si>
+  <si>
+    <t>PassedUpdating Object Properties</t>
+  </si>
+  <si>
+    <t>PassedAdd New Properties to a JavaScript Object</t>
+  </si>
+  <si>
+    <t>PassedDelete Properties from a JavaScript Object</t>
+  </si>
+  <si>
+    <t>PassedUsing Objects for Lookups</t>
+  </si>
+  <si>
+    <t>PassedTesting Objects for Properties</t>
+  </si>
+  <si>
+    <t>PassedManipulating Complex Objects</t>
+  </si>
+  <si>
+    <t>PassedAccessing Nested Objects</t>
+  </si>
+  <si>
+    <t>PassedAccessing Nested Arrays</t>
+  </si>
+  <si>
+    <t>PassedReturn Early Pattern for Functions</t>
   </si>
 </sst>
 </file>
@@ -1099,12 +1126,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1119,7 +1152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1136,6 +1169,7 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7581,8 +7615,8 @@
   <dimension ref="A1:F299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D81" sqref="D81:D85"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D94" sqref="D94:D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -8949,7 +8983,7 @@
         <v>79</v>
       </c>
       <c r="D80" t="s">
-        <v>79</v>
+        <v>354</v>
       </c>
       <c r="E80" s="2">
         <v>43432</v>
@@ -9051,7 +9085,7 @@
         <v>85</v>
       </c>
       <c r="D86" t="s">
-        <v>85</v>
+        <v>346</v>
       </c>
       <c r="E86" s="2">
         <v>43432</v>
@@ -9068,7 +9102,7 @@
         <v>86</v>
       </c>
       <c r="D87" t="s">
-        <v>86</v>
+        <v>347</v>
       </c>
       <c r="E87" s="2">
         <v>43432</v>
@@ -9085,7 +9119,7 @@
         <v>87</v>
       </c>
       <c r="D88" t="s">
-        <v>87</v>
+        <v>348</v>
       </c>
       <c r="E88" s="2">
         <v>43432</v>
@@ -9102,7 +9136,7 @@
         <v>88</v>
       </c>
       <c r="D89" t="s">
-        <v>88</v>
+        <v>349</v>
       </c>
       <c r="E89" s="2">
         <v>43432</v>
@@ -9119,7 +9153,7 @@
         <v>89</v>
       </c>
       <c r="D90" t="s">
-        <v>89</v>
+        <v>350</v>
       </c>
       <c r="E90" s="2">
         <v>43432</v>
@@ -9136,7 +9170,7 @@
         <v>90</v>
       </c>
       <c r="D91" t="s">
-        <v>90</v>
+        <v>351</v>
       </c>
       <c r="E91" s="2">
         <v>43432</v>
@@ -9153,7 +9187,7 @@
         <v>91</v>
       </c>
       <c r="D92" t="s">
-        <v>91</v>
+        <v>352</v>
       </c>
       <c r="E92" s="2">
         <v>43432</v>
@@ -9170,7 +9204,7 @@
         <v>92</v>
       </c>
       <c r="D93" t="s">
-        <v>92</v>
+        <v>353</v>
       </c>
       <c r="E93" s="2">
         <v>43432</v>
@@ -9186,7 +9220,7 @@
       <c r="C94" s="1">
         <v>93</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="8" t="s">
         <v>93</v>
       </c>
       <c r="E94" s="2">
@@ -9203,7 +9237,7 @@
       <c r="C95" s="1">
         <v>94</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="8" t="s">
         <v>94</v>
       </c>
       <c r="E95" s="2">
@@ -9220,7 +9254,7 @@
       <c r="C96" s="1">
         <v>95</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="8" t="s">
         <v>95</v>
       </c>
       <c r="E96" s="2">
@@ -9237,7 +9271,7 @@
       <c r="C97" s="1">
         <v>96</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="8" t="s">
         <v>96</v>
       </c>
       <c r="E97" s="2">
@@ -9257,7 +9291,7 @@
       <c r="C98" s="1">
         <v>97</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="8" t="s">
         <v>97</v>
       </c>
       <c r="E98" s="2">
@@ -9277,7 +9311,7 @@
       <c r="C99" s="1">
         <v>98</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="8" t="s">
         <v>98</v>
       </c>
       <c r="E99" s="2">
@@ -9297,7 +9331,7 @@
       <c r="C100" s="1">
         <v>99</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="8" t="s">
         <v>99</v>
       </c>
       <c r="E100" s="2">
@@ -9317,7 +9351,7 @@
       <c r="C101" s="1">
         <v>100</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="8" t="s">
         <v>100</v>
       </c>
       <c r="E101" s="2">
@@ -9337,7 +9371,7 @@
       <c r="C102" s="1">
         <v>101</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="8" t="s">
         <v>101</v>
       </c>
       <c r="E102" s="2">
@@ -9357,7 +9391,7 @@
       <c r="C103" s="1">
         <v>102</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="8" t="s">
         <v>102</v>
       </c>
       <c r="E103" s="2">
@@ -9377,7 +9411,7 @@
       <c r="C104" s="1">
         <v>103</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="8" t="s">
         <v>103</v>
       </c>
       <c r="E104" s="2">
@@ -9397,7 +9431,7 @@
       <c r="C105" s="1">
         <v>104</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="8" t="s">
         <v>104</v>
       </c>
       <c r="E105" s="2">
@@ -9417,7 +9451,7 @@
       <c r="C106" s="1">
         <v>105</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="8" t="s">
         <v>105</v>
       </c>
       <c r="E106" s="2">
@@ -9437,7 +9471,7 @@
       <c r="C107" s="1">
         <v>106</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="8" t="s">
         <v>106</v>
       </c>
       <c r="E107" s="2">
@@ -9457,7 +9491,7 @@
       <c r="C108" s="1">
         <v>107</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="8" t="s">
         <v>107</v>
       </c>
       <c r="E108" s="2">
@@ -9477,7 +9511,7 @@
       <c r="C109" s="1">
         <v>108</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="8" t="s">
         <v>108</v>
       </c>
       <c r="E109" s="2">
@@ -9497,7 +9531,7 @@
       <c r="C110" s="1">
         <v>109</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="8" t="s">
         <v>112</v>
       </c>
       <c r="E110" s="2">
@@ -9517,7 +9551,7 @@
       <c r="C111" s="1">
         <v>110</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="8" t="s">
         <v>113</v>
       </c>
       <c r="E111" s="2">
@@ -9537,7 +9571,7 @@
       <c r="C112" s="1">
         <v>111</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="8" t="s">
         <v>114</v>
       </c>
       <c r="E112" s="2">
@@ -9557,7 +9591,7 @@
       <c r="C113" s="1">
         <v>112</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="8" t="s">
         <v>115</v>
       </c>
       <c r="E113" s="2">
@@ -9577,7 +9611,7 @@
       <c r="C114" s="1">
         <v>113</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="8" t="s">
         <v>116</v>
       </c>
       <c r="E114" s="2">
@@ -9597,7 +9631,7 @@
       <c r="C115" s="1">
         <v>114</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" s="8" t="s">
         <v>117</v>
       </c>
       <c r="E115" s="2">
@@ -9617,7 +9651,7 @@
       <c r="C116" s="1">
         <v>115</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="8" t="s">
         <v>118</v>
       </c>
       <c r="E116" s="2">
@@ -9637,7 +9671,7 @@
       <c r="C117" s="1">
         <v>116</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" s="8" t="s">
         <v>119</v>
       </c>
       <c r="E117" s="2">
@@ -9657,7 +9691,7 @@
       <c r="C118" s="1">
         <v>117</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118" s="8" t="s">
         <v>120</v>
       </c>
       <c r="E118" s="2">
@@ -9677,7 +9711,7 @@
       <c r="C119" s="1">
         <v>118</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119" s="8" t="s">
         <v>121</v>
       </c>
       <c r="E119" s="2">
@@ -9697,7 +9731,7 @@
       <c r="C120" s="1">
         <v>119</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" s="8" t="s">
         <v>122</v>
       </c>
       <c r="E120" s="2">
@@ -9717,7 +9751,7 @@
       <c r="C121" s="1">
         <v>120</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" s="8" t="s">
         <v>123</v>
       </c>
       <c r="E121" s="2">
@@ -9737,7 +9771,7 @@
       <c r="C122" s="1">
         <v>121</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" s="8" t="s">
         <v>124</v>
       </c>
       <c r="E122" s="2">
@@ -9757,7 +9791,7 @@
       <c r="C123" s="1">
         <v>122</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123" s="8" t="s">
         <v>125</v>
       </c>
       <c r="E123" s="2">
@@ -9777,7 +9811,7 @@
       <c r="C124" s="1">
         <v>123</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D124" s="8" t="s">
         <v>126</v>
       </c>
       <c r="E124" s="2">
@@ -9797,7 +9831,7 @@
       <c r="C125" s="1">
         <v>124</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D125" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E125" s="2">
@@ -9817,7 +9851,7 @@
       <c r="C126" s="1">
         <v>125</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E126" s="2">
@@ -9837,7 +9871,7 @@
       <c r="C127" s="1">
         <v>126</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127" s="8" t="s">
         <v>129</v>
       </c>
       <c r="E127" s="2">
@@ -9857,7 +9891,7 @@
       <c r="C128" s="1">
         <v>127</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="8" t="s">
         <v>130</v>
       </c>
       <c r="E128" s="2">
@@ -9877,7 +9911,7 @@
       <c r="C129" s="1">
         <v>128</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="8" t="s">
         <v>131</v>
       </c>
       <c r="E129" s="2">
@@ -9897,7 +9931,7 @@
       <c r="C130" s="1">
         <v>129</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" s="8" t="s">
         <v>132</v>
       </c>
       <c r="E130" s="2">
@@ -9917,7 +9951,7 @@
       <c r="C131" s="1">
         <v>130</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D131" s="8" t="s">
         <v>133</v>
       </c>
       <c r="E131" s="2">
@@ -9937,7 +9971,7 @@
       <c r="C132" s="1">
         <v>131</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D132" s="8" t="s">
         <v>134</v>
       </c>
       <c r="E132" s="2">
@@ -9957,7 +9991,7 @@
       <c r="C133" s="1">
         <v>132</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D133" s="8" t="s">
         <v>135</v>
       </c>
       <c r="E133" s="2">
@@ -9977,7 +10011,7 @@
       <c r="C134" s="1">
         <v>133</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D134" s="8" t="s">
         <v>136</v>
       </c>
       <c r="E134" s="2">
@@ -9997,7 +10031,7 @@
       <c r="C135" s="1">
         <v>134</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D135" s="8" t="s">
         <v>137</v>
       </c>
       <c r="E135" s="2">
@@ -10017,7 +10051,7 @@
       <c r="C136" s="1">
         <v>135</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D136" s="8" t="s">
         <v>138</v>
       </c>
       <c r="E136" s="2">

</xml_diff>

<commit_message>
more loops and iteration
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB02C4A-A91C-4D4A-8DC1-3A7611BF6A24}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE8FC24-6875-4789-B1E9-93D4A5AE0A30}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="361">
   <si>
     <t>Basic JavaScript</t>
   </si>
@@ -1103,6 +1103,24 @@
   </si>
   <si>
     <t>PassedReturn Early Pattern for Functions</t>
+  </si>
+  <si>
+    <t>PassedRecord Collection</t>
+  </si>
+  <si>
+    <t>PassedIterate with JavaScript While Loops</t>
+  </si>
+  <si>
+    <t>PassedIterate with JavaScript For Loops</t>
+  </si>
+  <si>
+    <t>PassedIterate Odd Numbers With a For Loop</t>
+  </si>
+  <si>
+    <t>PassedCount Backwards With a For Loop</t>
+  </si>
+  <si>
+    <t>PassedIterate Through an Array with a For Loop</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1153,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1152,7 +1170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1169,6 +1187,8 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -7615,8 +7635,8 @@
   <dimension ref="A1:F299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D94" sqref="D94:D136"/>
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -9139,7 +9159,7 @@
         <v>349</v>
       </c>
       <c r="E89" s="2">
-        <v>43432</v>
+        <v>43433</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.75">
@@ -9156,7 +9176,7 @@
         <v>350</v>
       </c>
       <c r="E90" s="2">
-        <v>43432</v>
+        <v>43433</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.75">
@@ -9173,7 +9193,7 @@
         <v>351</v>
       </c>
       <c r="E91" s="2">
-        <v>43432</v>
+        <v>43433</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.75">
@@ -9190,7 +9210,7 @@
         <v>352</v>
       </c>
       <c r="E92" s="2">
-        <v>43432</v>
+        <v>43433</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.75">
@@ -9207,7 +9227,7 @@
         <v>353</v>
       </c>
       <c r="E93" s="2">
-        <v>43432</v>
+        <v>43433</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.75">
@@ -9221,10 +9241,10 @@
         <v>93</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>93</v>
+        <v>355</v>
       </c>
       <c r="E94" s="2">
-        <v>43432</v>
+        <v>43433</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.75">
@@ -9238,10 +9258,10 @@
         <v>94</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>94</v>
+        <v>356</v>
       </c>
       <c r="E95" s="2">
-        <v>43432</v>
+        <v>43433</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.75">
@@ -9255,10 +9275,10 @@
         <v>95</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>95</v>
+        <v>357</v>
       </c>
       <c r="E96" s="2">
-        <v>43432</v>
+        <v>43433</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.75">
@@ -9272,10 +9292,10 @@
         <v>96</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>96</v>
+        <v>358</v>
       </c>
       <c r="E97" s="2">
-        <v>43432</v>
+        <v>43433</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>335</v>
@@ -9292,10 +9312,10 @@
         <v>97</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>97</v>
+        <v>359</v>
       </c>
       <c r="E98" s="2">
-        <v>43432</v>
+        <v>43433</v>
       </c>
       <c r="F98" s="7" t="s">
         <v>335</v>
@@ -9311,10 +9331,10 @@
       <c r="C99" s="1">
         <v>98</v>
       </c>
-      <c r="D99" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="E99" s="2">
+      <c r="D99" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="E99" s="9">
         <v>43432</v>
       </c>
       <c r="F99" s="7" t="s">
@@ -9331,10 +9351,10 @@
       <c r="C100" s="1">
         <v>99</v>
       </c>
-      <c r="D100" s="8" t="s">
+      <c r="D100" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E100" s="2">
+      <c r="E100" s="9">
         <v>43432</v>
       </c>
       <c r="F100" s="7" t="s">
@@ -9351,10 +9371,10 @@
       <c r="C101" s="1">
         <v>100</v>
       </c>
-      <c r="D101" s="8" t="s">
+      <c r="D101" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E101" s="2">
+      <c r="E101" s="9">
         <v>43432</v>
       </c>
       <c r="F101" s="7" t="s">
@@ -9371,10 +9391,10 @@
       <c r="C102" s="1">
         <v>101</v>
       </c>
-      <c r="D102" s="8" t="s">
+      <c r="D102" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E102" s="2">
+      <c r="E102" s="9">
         <v>43432</v>
       </c>
       <c r="F102" s="7" t="s">
@@ -9391,10 +9411,10 @@
       <c r="C103" s="1">
         <v>102</v>
       </c>
-      <c r="D103" s="8" t="s">
+      <c r="D103" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E103" s="2">
+      <c r="E103" s="9">
         <v>43432</v>
       </c>
       <c r="F103" s="7" t="s">
@@ -9411,10 +9431,10 @@
       <c r="C104" s="1">
         <v>103</v>
       </c>
-      <c r="D104" s="8" t="s">
+      <c r="D104" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E104" s="2">
+      <c r="E104" s="9">
         <v>43432</v>
       </c>
       <c r="F104" s="7" t="s">
@@ -9431,10 +9451,10 @@
       <c r="C105" s="1">
         <v>104</v>
       </c>
-      <c r="D105" s="8" t="s">
+      <c r="D105" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E105" s="2">
+      <c r="E105" s="9">
         <v>43432</v>
       </c>
       <c r="F105" s="7" t="s">
@@ -9451,10 +9471,10 @@
       <c r="C106" s="1">
         <v>105</v>
       </c>
-      <c r="D106" s="8" t="s">
+      <c r="D106" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E106" s="2">
+      <c r="E106" s="9">
         <v>43432</v>
       </c>
       <c r="F106" s="7" t="s">
@@ -9471,10 +9491,10 @@
       <c r="C107" s="1">
         <v>106</v>
       </c>
-      <c r="D107" s="8" t="s">
+      <c r="D107" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E107" s="2">
+      <c r="E107" s="9">
         <v>43432</v>
       </c>
       <c r="F107" s="7" t="s">
@@ -9491,10 +9511,10 @@
       <c r="C108" s="1">
         <v>107</v>
       </c>
-      <c r="D108" s="8" t="s">
+      <c r="D108" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E108" s="2">
+      <c r="E108" s="9">
         <v>43432</v>
       </c>
       <c r="F108" s="7" t="s">
@@ -9511,10 +9531,10 @@
       <c r="C109" s="1">
         <v>108</v>
       </c>
-      <c r="D109" s="8" t="s">
+      <c r="D109" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E109" s="2">
+      <c r="E109" s="9">
         <v>43432</v>
       </c>
       <c r="F109" s="7" t="s">
@@ -9531,7 +9551,7 @@
       <c r="C110" s="1">
         <v>109</v>
       </c>
-      <c r="D110" s="8" t="s">
+      <c r="D110" s="10" t="s">
         <v>112</v>
       </c>
       <c r="E110" s="2">
@@ -9551,7 +9571,7 @@
       <c r="C111" s="1">
         <v>110</v>
       </c>
-      <c r="D111" s="8" t="s">
+      <c r="D111" s="10" t="s">
         <v>113</v>
       </c>
       <c r="E111" s="2">
@@ -9571,7 +9591,7 @@
       <c r="C112" s="1">
         <v>111</v>
       </c>
-      <c r="D112" s="8" t="s">
+      <c r="D112" s="10" t="s">
         <v>114</v>
       </c>
       <c r="E112" s="2">
@@ -9591,7 +9611,7 @@
       <c r="C113" s="1">
         <v>112</v>
       </c>
-      <c r="D113" s="8" t="s">
+      <c r="D113" s="10" t="s">
         <v>115</v>
       </c>
       <c r="E113" s="2">
@@ -9611,7 +9631,7 @@
       <c r="C114" s="1">
         <v>113</v>
       </c>
-      <c r="D114" s="8" t="s">
+      <c r="D114" s="10" t="s">
         <v>116</v>
       </c>
       <c r="E114" s="2">
@@ -9631,7 +9651,7 @@
       <c r="C115" s="1">
         <v>114</v>
       </c>
-      <c r="D115" s="8" t="s">
+      <c r="D115" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E115" s="2">
@@ -9651,7 +9671,7 @@
       <c r="C116" s="1">
         <v>115</v>
       </c>
-      <c r="D116" s="8" t="s">
+      <c r="D116" s="10" t="s">
         <v>118</v>
       </c>
       <c r="E116" s="2">
@@ -9671,7 +9691,7 @@
       <c r="C117" s="1">
         <v>116</v>
       </c>
-      <c r="D117" s="8" t="s">
+      <c r="D117" s="10" t="s">
         <v>119</v>
       </c>
       <c r="E117" s="2">
@@ -9691,7 +9711,7 @@
       <c r="C118" s="1">
         <v>117</v>
       </c>
-      <c r="D118" s="8" t="s">
+      <c r="D118" s="10" t="s">
         <v>120</v>
       </c>
       <c r="E118" s="2">
@@ -9711,7 +9731,7 @@
       <c r="C119" s="1">
         <v>118</v>
       </c>
-      <c r="D119" s="8" t="s">
+      <c r="D119" s="10" t="s">
         <v>121</v>
       </c>
       <c r="E119" s="2">
@@ -9731,7 +9751,7 @@
       <c r="C120" s="1">
         <v>119</v>
       </c>
-      <c r="D120" s="8" t="s">
+      <c r="D120" s="10" t="s">
         <v>122</v>
       </c>
       <c r="E120" s="2">
@@ -9751,7 +9771,7 @@
       <c r="C121" s="1">
         <v>120</v>
       </c>
-      <c r="D121" s="8" t="s">
+      <c r="D121" s="10" t="s">
         <v>123</v>
       </c>
       <c r="E121" s="2">
@@ -9771,7 +9791,7 @@
       <c r="C122" s="1">
         <v>121</v>
       </c>
-      <c r="D122" s="8" t="s">
+      <c r="D122" s="10" t="s">
         <v>124</v>
       </c>
       <c r="E122" s="2">
@@ -9791,7 +9811,7 @@
       <c r="C123" s="1">
         <v>122</v>
       </c>
-      <c r="D123" s="8" t="s">
+      <c r="D123" s="10" t="s">
         <v>125</v>
       </c>
       <c r="E123" s="2">
@@ -9811,7 +9831,7 @@
       <c r="C124" s="1">
         <v>123</v>
       </c>
-      <c r="D124" s="8" t="s">
+      <c r="D124" s="10" t="s">
         <v>126</v>
       </c>
       <c r="E124" s="2">
@@ -9831,7 +9851,7 @@
       <c r="C125" s="1">
         <v>124</v>
       </c>
-      <c r="D125" s="8" t="s">
+      <c r="D125" s="10" t="s">
         <v>127</v>
       </c>
       <c r="E125" s="2">
@@ -9851,7 +9871,7 @@
       <c r="C126" s="1">
         <v>125</v>
       </c>
-      <c r="D126" s="8" t="s">
+      <c r="D126" s="10" t="s">
         <v>128</v>
       </c>
       <c r="E126" s="2">
@@ -9871,7 +9891,7 @@
       <c r="C127" s="1">
         <v>126</v>
       </c>
-      <c r="D127" s="8" t="s">
+      <c r="D127" s="10" t="s">
         <v>129</v>
       </c>
       <c r="E127" s="2">
@@ -9891,7 +9911,7 @@
       <c r="C128" s="1">
         <v>127</v>
       </c>
-      <c r="D128" s="8" t="s">
+      <c r="D128" s="10" t="s">
         <v>130</v>
       </c>
       <c r="E128" s="2">
@@ -9911,7 +9931,7 @@
       <c r="C129" s="1">
         <v>128</v>
       </c>
-      <c r="D129" s="8" t="s">
+      <c r="D129" s="10" t="s">
         <v>131</v>
       </c>
       <c r="E129" s="2">
@@ -9931,7 +9951,7 @@
       <c r="C130" s="1">
         <v>129</v>
       </c>
-      <c r="D130" s="8" t="s">
+      <c r="D130" s="10" t="s">
         <v>132</v>
       </c>
       <c r="E130" s="2">
@@ -9951,7 +9971,7 @@
       <c r="C131" s="1">
         <v>130</v>
       </c>
-      <c r="D131" s="8" t="s">
+      <c r="D131" s="10" t="s">
         <v>133</v>
       </c>
       <c r="E131" s="2">
@@ -9971,7 +9991,7 @@
       <c r="C132" s="1">
         <v>131</v>
       </c>
-      <c r="D132" s="8" t="s">
+      <c r="D132" s="10" t="s">
         <v>134</v>
       </c>
       <c r="E132" s="2">
@@ -9991,7 +10011,7 @@
       <c r="C133" s="1">
         <v>132</v>
       </c>
-      <c r="D133" s="8" t="s">
+      <c r="D133" s="10" t="s">
         <v>135</v>
       </c>
       <c r="E133" s="2">
@@ -10011,7 +10031,7 @@
       <c r="C134" s="1">
         <v>133</v>
       </c>
-      <c r="D134" s="8" t="s">
+      <c r="D134" s="10" t="s">
         <v>136</v>
       </c>
       <c r="E134" s="2">
@@ -10031,7 +10051,7 @@
       <c r="C135" s="1">
         <v>134</v>
       </c>
-      <c r="D135" s="8" t="s">
+      <c r="D135" s="10" t="s">
         <v>137</v>
       </c>
       <c r="E135" s="2">
@@ -10051,7 +10071,7 @@
       <c r="C136" s="1">
         <v>135</v>
       </c>
-      <c r="D136" s="8" t="s">
+      <c r="D136" s="10" t="s">
         <v>138</v>
       </c>
       <c r="E136" s="2">
@@ -10071,7 +10091,7 @@
       <c r="C137" s="1">
         <v>136</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D137" s="10" t="s">
         <v>140</v>
       </c>
       <c r="E137" s="2">
@@ -10091,7 +10111,7 @@
       <c r="C138" s="1">
         <v>137</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D138" s="10" t="s">
         <v>141</v>
       </c>
       <c r="E138" s="2">

</xml_diff>

<commit_message>
Basic JavaScript complete Tertiary Conditionals
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE8FC24-6875-4789-B1E9-93D4A5AE0A30}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26C4725-22DD-4C91-85B8-84F474FB1424}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1970" uniqueCount="368">
   <si>
     <t>Basic JavaScript</t>
   </si>
@@ -1121,6 +1121,27 @@
   </si>
   <si>
     <t>PassedIterate Through an Array with a For Loop</t>
+  </si>
+  <si>
+    <t>PassedNesting For Loops</t>
+  </si>
+  <si>
+    <t>PassedIterate with JavaScript Do...While Loops</t>
+  </si>
+  <si>
+    <t>PassedProfile Lookup</t>
+  </si>
+  <si>
+    <t>PassedGenerate Random Fractions with JavaScript</t>
+  </si>
+  <si>
+    <t>PassedGenerate Random Whole Numbers with JavaScript</t>
+  </si>
+  <si>
+    <t>PassedGenerate Random Whole Numbers within a Range</t>
+  </si>
+  <si>
+    <t>PassedUse the parseInt Function</t>
   </si>
 </sst>
 </file>
@@ -7635,8 +7656,8 @@
   <dimension ref="A1:F299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D137" sqref="D137"/>
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D98" sqref="D98:D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -9331,7 +9352,7 @@
       <c r="C99" s="1">
         <v>98</v>
       </c>
-      <c r="D99" s="10" t="s">
+      <c r="D99" s="8" t="s">
         <v>360</v>
       </c>
       <c r="E99" s="9">
@@ -9351,8 +9372,8 @@
       <c r="C100" s="1">
         <v>99</v>
       </c>
-      <c r="D100" s="10" t="s">
-        <v>99</v>
+      <c r="D100" s="8" t="s">
+        <v>361</v>
       </c>
       <c r="E100" s="9">
         <v>43432</v>
@@ -9371,8 +9392,8 @@
       <c r="C101" s="1">
         <v>100</v>
       </c>
-      <c r="D101" s="10" t="s">
-        <v>100</v>
+      <c r="D101" s="8" t="s">
+        <v>362</v>
       </c>
       <c r="E101" s="9">
         <v>43432</v>
@@ -9391,8 +9412,8 @@
       <c r="C102" s="1">
         <v>101</v>
       </c>
-      <c r="D102" s="10" t="s">
-        <v>101</v>
+      <c r="D102" s="8" t="s">
+        <v>363</v>
       </c>
       <c r="E102" s="9">
         <v>43432</v>
@@ -9411,8 +9432,8 @@
       <c r="C103" s="1">
         <v>102</v>
       </c>
-      <c r="D103" s="10" t="s">
-        <v>102</v>
+      <c r="D103" s="8" t="s">
+        <v>364</v>
       </c>
       <c r="E103" s="9">
         <v>43432</v>
@@ -9431,8 +9452,8 @@
       <c r="C104" s="1">
         <v>103</v>
       </c>
-      <c r="D104" s="10" t="s">
-        <v>103</v>
+      <c r="D104" s="8" t="s">
+        <v>365</v>
       </c>
       <c r="E104" s="9">
         <v>43432</v>
@@ -9451,8 +9472,8 @@
       <c r="C105" s="1">
         <v>104</v>
       </c>
-      <c r="D105" s="10" t="s">
-        <v>104</v>
+      <c r="D105" s="8" t="s">
+        <v>366</v>
       </c>
       <c r="E105" s="9">
         <v>43432</v>
@@ -9471,8 +9492,8 @@
       <c r="C106" s="1">
         <v>105</v>
       </c>
-      <c r="D106" s="10" t="s">
-        <v>105</v>
+      <c r="D106" s="8" t="s">
+        <v>367</v>
       </c>
       <c r="E106" s="9">
         <v>43432</v>

</xml_diff>

<commit_message>
ES6 Let vs Var Scope
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26C4725-22DD-4C91-85B8-84F474FB1424}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75012570-E83F-43C8-A1F7-DEBB01C0A196}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1970" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="373">
   <si>
     <t>Basic JavaScript</t>
   </si>
@@ -1142,6 +1142,21 @@
   </si>
   <si>
     <t>PassedUse the parseInt Function</t>
+  </si>
+  <si>
+    <t>PassedUse the parseInt Function with a Radix</t>
+  </si>
+  <si>
+    <t>PassedUse the Conditional (Ternary) Operator</t>
+  </si>
+  <si>
+    <t>PassedUse Multiple Conditional (Ternary) Operators</t>
+  </si>
+  <si>
+    <t>PassedExplore Differences Between the var and let Keywords</t>
+  </si>
+  <si>
+    <t>PassedCompare Scopes of the var and let Keywords</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1230,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7656,8 +7691,8 @@
   <dimension ref="A1:F299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D98" sqref="D98:D106"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -9512,8 +9547,8 @@
       <c r="C107" s="1">
         <v>106</v>
       </c>
-      <c r="D107" s="10" t="s">
-        <v>106</v>
+      <c r="D107" s="8" t="s">
+        <v>368</v>
       </c>
       <c r="E107" s="9">
         <v>43432</v>
@@ -9532,8 +9567,8 @@
       <c r="C108" s="1">
         <v>107</v>
       </c>
-      <c r="D108" s="10" t="s">
-        <v>107</v>
+      <c r="D108" s="8" t="s">
+        <v>369</v>
       </c>
       <c r="E108" s="9">
         <v>43432</v>
@@ -9552,8 +9587,8 @@
       <c r="C109" s="1">
         <v>108</v>
       </c>
-      <c r="D109" s="10" t="s">
-        <v>108</v>
+      <c r="D109" s="8" t="s">
+        <v>370</v>
       </c>
       <c r="E109" s="9">
         <v>43432</v>
@@ -9570,9 +9605,9 @@
         <v>111</v>
       </c>
       <c r="C110" s="1">
-        <v>109</v>
-      </c>
-      <c r="D110" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D110" s="8" t="s">
         <v>112</v>
       </c>
       <c r="E110" s="2">
@@ -9590,10 +9625,10 @@
         <v>111</v>
       </c>
       <c r="C111" s="1">
-        <v>110</v>
-      </c>
-      <c r="D111" s="10" t="s">
-        <v>113</v>
+        <v>2</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>371</v>
       </c>
       <c r="E111" s="2">
         <v>43432</v>
@@ -9610,10 +9645,10 @@
         <v>111</v>
       </c>
       <c r="C112" s="1">
-        <v>111</v>
-      </c>
-      <c r="D112" s="10" t="s">
-        <v>114</v>
+        <v>3</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>372</v>
       </c>
       <c r="E112" s="2">
         <v>43432</v>
@@ -9630,7 +9665,7 @@
         <v>111</v>
       </c>
       <c r="C113" s="1">
-        <v>112</v>
+        <v>4</v>
       </c>
       <c r="D113" s="10" t="s">
         <v>115</v>
@@ -9650,7 +9685,7 @@
         <v>111</v>
       </c>
       <c r="C114" s="1">
-        <v>113</v>
+        <v>5</v>
       </c>
       <c r="D114" s="10" t="s">
         <v>116</v>
@@ -9670,7 +9705,7 @@
         <v>111</v>
       </c>
       <c r="C115" s="1">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="D115" s="10" t="s">
         <v>117</v>
@@ -9690,7 +9725,7 @@
         <v>111</v>
       </c>
       <c r="C116" s="1">
-        <v>115</v>
+        <v>7</v>
       </c>
       <c r="D116" s="10" t="s">
         <v>118</v>
@@ -9710,7 +9745,7 @@
         <v>111</v>
       </c>
       <c r="C117" s="1">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="D117" s="10" t="s">
         <v>119</v>
@@ -9730,7 +9765,7 @@
         <v>111</v>
       </c>
       <c r="C118" s="1">
-        <v>117</v>
+        <v>9</v>
       </c>
       <c r="D118" s="10" t="s">
         <v>120</v>
@@ -9750,7 +9785,7 @@
         <v>111</v>
       </c>
       <c r="C119" s="1">
-        <v>118</v>
+        <v>10</v>
       </c>
       <c r="D119" s="10" t="s">
         <v>121</v>
@@ -9770,7 +9805,7 @@
         <v>111</v>
       </c>
       <c r="C120" s="1">
-        <v>119</v>
+        <v>11</v>
       </c>
       <c r="D120" s="10" t="s">
         <v>122</v>
@@ -9790,7 +9825,7 @@
         <v>111</v>
       </c>
       <c r="C121" s="1">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="D121" s="10" t="s">
         <v>123</v>
@@ -9810,7 +9845,7 @@
         <v>111</v>
       </c>
       <c r="C122" s="1">
-        <v>121</v>
+        <v>13</v>
       </c>
       <c r="D122" s="10" t="s">
         <v>124</v>
@@ -9830,7 +9865,7 @@
         <v>111</v>
       </c>
       <c r="C123" s="1">
-        <v>122</v>
+        <v>14</v>
       </c>
       <c r="D123" s="10" t="s">
         <v>125</v>
@@ -9850,7 +9885,7 @@
         <v>111</v>
       </c>
       <c r="C124" s="1">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="D124" s="10" t="s">
         <v>126</v>
@@ -9870,7 +9905,7 @@
         <v>111</v>
       </c>
       <c r="C125" s="1">
-        <v>124</v>
+        <v>16</v>
       </c>
       <c r="D125" s="10" t="s">
         <v>127</v>
@@ -9890,7 +9925,7 @@
         <v>111</v>
       </c>
       <c r="C126" s="1">
-        <v>125</v>
+        <v>17</v>
       </c>
       <c r="D126" s="10" t="s">
         <v>128</v>
@@ -9910,7 +9945,7 @@
         <v>111</v>
       </c>
       <c r="C127" s="1">
-        <v>126</v>
+        <v>18</v>
       </c>
       <c r="D127" s="10" t="s">
         <v>129</v>
@@ -9930,7 +9965,7 @@
         <v>111</v>
       </c>
       <c r="C128" s="1">
-        <v>127</v>
+        <v>19</v>
       </c>
       <c r="D128" s="10" t="s">
         <v>130</v>
@@ -9950,7 +9985,7 @@
         <v>111</v>
       </c>
       <c r="C129" s="1">
-        <v>128</v>
+        <v>20</v>
       </c>
       <c r="D129" s="10" t="s">
         <v>131</v>
@@ -9970,7 +10005,7 @@
         <v>111</v>
       </c>
       <c r="C130" s="1">
-        <v>129</v>
+        <v>21</v>
       </c>
       <c r="D130" s="10" t="s">
         <v>132</v>
@@ -9990,7 +10025,7 @@
         <v>111</v>
       </c>
       <c r="C131" s="1">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="D131" s="10" t="s">
         <v>133</v>
@@ -10010,7 +10045,7 @@
         <v>111</v>
       </c>
       <c r="C132" s="1">
-        <v>131</v>
+        <v>23</v>
       </c>
       <c r="D132" s="10" t="s">
         <v>134</v>
@@ -10030,7 +10065,7 @@
         <v>111</v>
       </c>
       <c r="C133" s="1">
-        <v>132</v>
+        <v>24</v>
       </c>
       <c r="D133" s="10" t="s">
         <v>135</v>
@@ -10050,7 +10085,7 @@
         <v>111</v>
       </c>
       <c r="C134" s="1">
-        <v>133</v>
+        <v>25</v>
       </c>
       <c r="D134" s="10" t="s">
         <v>136</v>
@@ -10070,7 +10105,7 @@
         <v>111</v>
       </c>
       <c r="C135" s="1">
-        <v>134</v>
+        <v>26</v>
       </c>
       <c r="D135" s="10" t="s">
         <v>137</v>
@@ -10090,7 +10125,7 @@
         <v>111</v>
       </c>
       <c r="C136" s="1">
-        <v>135</v>
+        <v>27</v>
       </c>
       <c r="D136" s="10" t="s">
         <v>138</v>
@@ -10112,7 +10147,7 @@
       <c r="C137" s="1">
         <v>136</v>
       </c>
-      <c r="D137" s="10" t="s">
+      <c r="D137" s="8" t="s">
         <v>140</v>
       </c>
       <c r="E137" s="2">
@@ -10132,7 +10167,7 @@
       <c r="C138" s="1">
         <v>137</v>
       </c>
-      <c r="D138" s="10" t="s">
+      <c r="D138" s="8" t="s">
         <v>141</v>
       </c>
       <c r="E138" s="2">
@@ -13368,11 +13403,8 @@
     <sortCondition ref="A2:A317"/>
     <sortCondition ref="C2:C317"/>
   </sortState>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>43428</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
JS ES6: Use Destructuring Assignment to Assign Variables from Objects
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151A5768-5C52-41A3-8B92-11E5399E7FD6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C6ACE3-67AE-40B6-BB52-FB323DB670DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="386">
   <si>
     <t>Basic JavaScript</t>
   </si>
@@ -1166,6 +1166,36 @@
   </si>
   <si>
     <t>2,080 hours = 208 days. FOR ENTIRE FCC &amp; ALL CERTIFICATIONS</t>
+  </si>
+  <si>
+    <t>PassedDeclare a Read-Only Variable with the const Keyword</t>
+  </si>
+  <si>
+    <t>PassedMutate an Array Declared with const</t>
+  </si>
+  <si>
+    <t>PassedPrevent Object Mutation</t>
+  </si>
+  <si>
+    <t>PassedUse Arrow Functions to Write Concise Anonymous Functions</t>
+  </si>
+  <si>
+    <t>PassedWrite Arrow Functions with Parameters</t>
+  </si>
+  <si>
+    <t>PassedWrite Higher Order Arrow Functions</t>
+  </si>
+  <si>
+    <t>PassedSet Default Parameters for Your Functions</t>
+  </si>
+  <si>
+    <t>PassedUse the Rest Operator with Function Parameters</t>
+  </si>
+  <si>
+    <t>PassedUse the Spread Operator to Evaluate Arrays In-Place</t>
+  </si>
+  <si>
+    <t>PassedUse Destructuring Assignment to Assign Variables from Objects</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1234,6 +1264,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7669,8 +7700,8 @@
   <dimension ref="A1:G302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D301" sqref="D301"/>
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -9599,11 +9630,11 @@
       <c r="C113" s="1">
         <v>4</v>
       </c>
-      <c r="D113" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>373</v>
+      <c r="D113" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="E113" s="2">
+        <v>43436</v>
       </c>
       <c r="F113" s="7">
         <v>43426</v>
@@ -9622,11 +9653,11 @@
       <c r="C114" s="1">
         <v>5</v>
       </c>
-      <c r="D114" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>373</v>
+      <c r="D114" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="E114" s="2">
+        <v>43436</v>
       </c>
       <c r="G114">
         <f>G113-F113</f>
@@ -9643,11 +9674,11 @@
       <c r="C115" s="1">
         <v>6</v>
       </c>
-      <c r="D115" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>373</v>
+      <c r="D115" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E115" s="2">
+        <v>43436</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.75">
@@ -9660,11 +9691,11 @@
       <c r="C116" s="1">
         <v>7</v>
       </c>
-      <c r="D116" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>373</v>
+      <c r="D116" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="E116" s="2">
+        <v>43436</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.75">
@@ -9677,11 +9708,11 @@
       <c r="C117" s="1">
         <v>8</v>
       </c>
-      <c r="D117" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>373</v>
+      <c r="D117" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="E117" s="2">
+        <v>43436</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.75">
@@ -9694,11 +9725,11 @@
       <c r="C118" s="1">
         <v>9</v>
       </c>
-      <c r="D118" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>373</v>
+      <c r="D118" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="E118" s="2">
+        <v>43436</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.75">
@@ -9711,11 +9742,11 @@
       <c r="C119" s="1">
         <v>10</v>
       </c>
-      <c r="D119" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E119" s="2" t="s">
-        <v>373</v>
+      <c r="D119" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="E119" s="2">
+        <v>43436</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.75">
@@ -9728,11 +9759,11 @@
       <c r="C120" s="1">
         <v>11</v>
       </c>
-      <c r="D120" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>373</v>
+      <c r="D120" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="E120" s="2">
+        <v>43436</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.75">
@@ -9745,11 +9776,11 @@
       <c r="C121" s="1">
         <v>12</v>
       </c>
-      <c r="D121" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>373</v>
+      <c r="D121" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="E121" s="2">
+        <v>43436</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.75">
@@ -9762,11 +9793,11 @@
       <c r="C122" s="1">
         <v>13</v>
       </c>
-      <c r="D122" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="E122" s="2" t="s">
-        <v>373</v>
+      <c r="D122" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="E122" s="2">
+        <v>43436</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.75">
@@ -9779,7 +9810,7 @@
       <c r="C123" s="1">
         <v>14</v>
       </c>
-      <c r="D123" s="9" t="s">
+      <c r="D123" s="10" t="s">
         <v>125</v>
       </c>
       <c r="E123" s="2" t="s">
@@ -9796,7 +9827,7 @@
       <c r="C124" s="1">
         <v>15</v>
       </c>
-      <c r="D124" s="9" t="s">
+      <c r="D124" s="10" t="s">
         <v>126</v>
       </c>
       <c r="E124" s="2" t="s">
@@ -9813,7 +9844,7 @@
       <c r="C125" s="1">
         <v>16</v>
       </c>
-      <c r="D125" s="9" t="s">
+      <c r="D125" s="10" t="s">
         <v>127</v>
       </c>
       <c r="E125" s="2" t="s">
@@ -9830,7 +9861,7 @@
       <c r="C126" s="1">
         <v>17</v>
       </c>
-      <c r="D126" s="9" t="s">
+      <c r="D126" s="10" t="s">
         <v>128</v>
       </c>
       <c r="E126" s="2" t="s">
@@ -9847,7 +9878,7 @@
       <c r="C127" s="1">
         <v>18</v>
       </c>
-      <c r="D127" s="9" t="s">
+      <c r="D127" s="10" t="s">
         <v>129</v>
       </c>
       <c r="E127" s="2" t="s">
@@ -9864,7 +9895,7 @@
       <c r="C128" s="1">
         <v>19</v>
       </c>
-      <c r="D128" s="9" t="s">
+      <c r="D128" s="10" t="s">
         <v>130</v>
       </c>
       <c r="E128" s="2" t="s">
@@ -9881,7 +9912,7 @@
       <c r="C129" s="1">
         <v>20</v>
       </c>
-      <c r="D129" s="9" t="s">
+      <c r="D129" s="10" t="s">
         <v>131</v>
       </c>
       <c r="E129" s="2" t="s">
@@ -9898,7 +9929,7 @@
       <c r="C130" s="1">
         <v>21</v>
       </c>
-      <c r="D130" s="9" t="s">
+      <c r="D130" s="10" t="s">
         <v>132</v>
       </c>
       <c r="E130" s="2" t="s">
@@ -9915,7 +9946,7 @@
       <c r="C131" s="1">
         <v>22</v>
       </c>
-      <c r="D131" s="9" t="s">
+      <c r="D131" s="10" t="s">
         <v>133</v>
       </c>
       <c r="E131" s="2" t="s">
@@ -9932,7 +9963,7 @@
       <c r="C132" s="1">
         <v>23</v>
       </c>
-      <c r="D132" s="9" t="s">
+      <c r="D132" s="10" t="s">
         <v>134</v>
       </c>
       <c r="E132" s="2" t="s">

</xml_diff>

<commit_message>
ES6 Class Syntax and Constructors
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C6ACE3-67AE-40B6-BB52-FB323DB670DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D834F348-8642-4034-8F49-CCBF51F70D3A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="392">
   <si>
     <t>Basic JavaScript</t>
   </si>
@@ -1196,6 +1196,24 @@
   </si>
   <si>
     <t>PassedUse Destructuring Assignment to Assign Variables from Objects</t>
+  </si>
+  <si>
+    <t>PassedUse Destructuring Assignment to Assign Variables from Nested Objects</t>
+  </si>
+  <si>
+    <t>PassedUse Destructuring Assignment to Assign Variables from Arrays</t>
+  </si>
+  <si>
+    <t>PassedUse Destructuring Assignment with the Rest Operator to Reassign Array Elements</t>
+  </si>
+  <si>
+    <t>PassedUse Destructuring Assignment to Pass an Object as a Function's Parameters</t>
+  </si>
+  <si>
+    <t>PassedCreate Strings using Template Literals</t>
+  </si>
+  <si>
+    <t>PassedWrite Concise Object Literal Declarations Using Simple Fields</t>
   </si>
 </sst>
 </file>
@@ -1219,7 +1237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1229,6 +1247,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1245,7 +1269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1264,7 +1288,8 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7701,7 +7726,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D121" sqref="D121"/>
+      <selection pane="bottomLeft" activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -9810,11 +9835,11 @@
       <c r="C123" s="1">
         <v>14</v>
       </c>
-      <c r="D123" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="E123" s="2" t="s">
-        <v>373</v>
+      <c r="D123" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="E123" s="2">
+        <v>43437</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.75">
@@ -9827,11 +9852,11 @@
       <c r="C124" s="1">
         <v>15</v>
       </c>
-      <c r="D124" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E124" s="2" t="s">
-        <v>373</v>
+      <c r="D124" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="E124" s="2">
+        <v>43437</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.75">
@@ -9844,11 +9869,11 @@
       <c r="C125" s="1">
         <v>16</v>
       </c>
-      <c r="D125" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>373</v>
+      <c r="D125" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="E125" s="2">
+        <v>43437</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.75">
@@ -9861,11 +9886,11 @@
       <c r="C126" s="1">
         <v>17</v>
       </c>
-      <c r="D126" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E126" s="2" t="s">
-        <v>373</v>
+      <c r="D126" s="11" t="s">
+        <v>389</v>
+      </c>
+      <c r="E126" s="2">
+        <v>43437</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.75">
@@ -9878,11 +9903,11 @@
       <c r="C127" s="1">
         <v>18</v>
       </c>
-      <c r="D127" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>373</v>
+      <c r="D127" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="E127" s="2">
+        <v>43437</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.75">
@@ -9895,11 +9920,11 @@
       <c r="C128" s="1">
         <v>19</v>
       </c>
-      <c r="D128" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>373</v>
+      <c r="D128" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="E128" s="2">
+        <v>43437</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.75">
@@ -9912,11 +9937,11 @@
       <c r="C129" s="1">
         <v>20</v>
       </c>
-      <c r="D129" s="10" t="s">
+      <c r="D129" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E129" s="2" t="s">
-        <v>373</v>
+      <c r="E129" s="2">
+        <v>43437</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.75">
@@ -9929,11 +9954,11 @@
       <c r="C130" s="1">
         <v>21</v>
       </c>
-      <c r="D130" s="10" t="s">
+      <c r="D130" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="E130" s="2" t="s">
-        <v>373</v>
+      <c r="E130" s="2">
+        <v>43437</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
ES6 import file using *
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E297B73-F77A-4C55-82E7-B7910FBB486C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DE8871-885E-49C0-B454-EDE9854371CE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2084" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3089" uniqueCount="397">
   <si>
     <t>Basic JavaScript</t>
   </si>
@@ -1226,6 +1226,9 @@
   </si>
   <si>
     <t>PassedUnderstand the Differences Between import and require</t>
+  </si>
+  <si>
+    <t>PassedUse export to Reuse a Code Block</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1261,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1275,7 +1278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1293,9 +1296,8 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7731,8 +7733,8 @@
   <dimension ref="A1:G302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E133" sqref="E133"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -9841,7 +9843,7 @@
       <c r="C123" s="1">
         <v>14</v>
       </c>
-      <c r="D123" s="10" t="s">
+      <c r="D123" s="9" t="s">
         <v>386</v>
       </c>
       <c r="E123" s="2">
@@ -9858,7 +9860,7 @@
       <c r="C124" s="1">
         <v>15</v>
       </c>
-      <c r="D124" s="10" t="s">
+      <c r="D124" s="9" t="s">
         <v>387</v>
       </c>
       <c r="E124" s="2">
@@ -9875,7 +9877,7 @@
       <c r="C125" s="1">
         <v>16</v>
       </c>
-      <c r="D125" s="10" t="s">
+      <c r="D125" s="9" t="s">
         <v>388</v>
       </c>
       <c r="E125" s="2">
@@ -9892,7 +9894,7 @@
       <c r="C126" s="1">
         <v>17</v>
       </c>
-      <c r="D126" s="10" t="s">
+      <c r="D126" s="9" t="s">
         <v>389</v>
       </c>
       <c r="E126" s="2">
@@ -9909,7 +9911,7 @@
       <c r="C127" s="1">
         <v>18</v>
       </c>
-      <c r="D127" s="10" t="s">
+      <c r="D127" s="9" t="s">
         <v>390</v>
       </c>
       <c r="E127" s="2">
@@ -9926,7 +9928,7 @@
       <c r="C128" s="1">
         <v>19</v>
       </c>
-      <c r="D128" s="10" t="s">
+      <c r="D128" s="9" t="s">
         <v>391</v>
       </c>
       <c r="E128" s="2">
@@ -9943,7 +9945,7 @@
       <c r="C129" s="1">
         <v>20</v>
       </c>
-      <c r="D129" s="10" t="s">
+      <c r="D129" s="9" t="s">
         <v>392</v>
       </c>
       <c r="E129" s="2">
@@ -9960,7 +9962,7 @@
       <c r="C130" s="1">
         <v>21</v>
       </c>
-      <c r="D130" s="10" t="s">
+      <c r="D130" s="9" t="s">
         <v>393</v>
       </c>
       <c r="E130" s="2">
@@ -9977,7 +9979,7 @@
       <c r="C131" s="1">
         <v>22</v>
       </c>
-      <c r="D131" s="11" t="s">
+      <c r="D131" s="9" t="s">
         <v>394</v>
       </c>
       <c r="E131" s="2">
@@ -9994,7 +9996,7 @@
       <c r="C132" s="1">
         <v>23</v>
       </c>
-      <c r="D132" s="11" t="s">
+      <c r="D132" s="9" t="s">
         <v>395</v>
       </c>
       <c r="E132" s="2">
@@ -10012,10 +10014,10 @@
         <v>24</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="E133" s="2" t="s">
-        <v>373</v>
+        <v>396</v>
+      </c>
+      <c r="E133" s="2">
+        <v>43437</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.75">
@@ -10028,7 +10030,7 @@
       <c r="C134" s="1">
         <v>25</v>
       </c>
-      <c r="D134" s="9" t="s">
+      <c r="D134" s="10" t="s">
         <v>136</v>
       </c>
       <c r="E134" s="2" t="s">
@@ -10045,7 +10047,7 @@
       <c r="C135" s="1">
         <v>26</v>
       </c>
-      <c r="D135" s="9" t="s">
+      <c r="D135" s="10" t="s">
         <v>137</v>
       </c>
       <c r="E135" s="2" t="s">
@@ -10062,7 +10064,7 @@
       <c r="C136" s="1">
         <v>27</v>
       </c>
-      <c r="D136" s="9" t="s">
+      <c r="D136" s="10" t="s">
         <v>138</v>
       </c>
       <c r="E136" s="2" t="s">
@@ -10079,7 +10081,7 @@
       <c r="C137" s="1">
         <v>136</v>
       </c>
-      <c r="D137" s="8" t="s">
+      <c r="D137" s="10" t="s">
         <v>140</v>
       </c>
       <c r="E137" s="2" t="s">
@@ -10096,7 +10098,7 @@
       <c r="C138" s="1">
         <v>137</v>
       </c>
-      <c r="D138" s="8" t="s">
+      <c r="D138" s="10" t="s">
         <v>141</v>
       </c>
       <c r="E138" s="2" t="s">
@@ -10113,7 +10115,7 @@
       <c r="C139" s="1">
         <v>138</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D139" s="10" t="s">
         <v>142</v>
       </c>
       <c r="E139" s="2" t="s">
@@ -10130,7 +10132,7 @@
       <c r="C140" s="1">
         <v>139</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D140" s="10" t="s">
         <v>143</v>
       </c>
       <c r="E140" s="2" t="s">
@@ -10147,7 +10149,7 @@
       <c r="C141" s="1">
         <v>140</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D141" s="10" t="s">
         <v>144</v>
       </c>
       <c r="E141" s="2" t="s">
@@ -10164,7 +10166,7 @@
       <c r="C142" s="1">
         <v>141</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D142" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E142" s="2" t="s">
@@ -10181,7 +10183,7 @@
       <c r="C143" s="1">
         <v>142</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143" s="10" t="s">
         <v>146</v>
       </c>
       <c r="E143" s="2" t="s">

</xml_diff>

<commit_message>
Regex negated character sets
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75920905-3834-4CEA-9659-6534EAD33866}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0CBD21-B43E-4243-92D0-685C0BFDB981}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
@@ -1279,7 +1279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1289,6 +1289,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1305,7 +1311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1326,6 +1332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7761,8 +7768,8 @@
   <dimension ref="A1:H302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D143" sqref="D143"/>
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -10253,7 +10260,7 @@
       <c r="D144" s="1">
         <v>8</v>
       </c>
-      <c r="E144" s="10" t="s">
+      <c r="E144" s="12" t="s">
         <v>147</v>
       </c>
       <c r="F144" s="11">
@@ -10273,7 +10280,7 @@
       <c r="D145" s="1">
         <v>9</v>
       </c>
-      <c r="E145" s="10" t="s">
+      <c r="E145" s="12" t="s">
         <v>148</v>
       </c>
       <c r="F145" s="11">
@@ -10293,7 +10300,7 @@
       <c r="D146" s="1">
         <v>10</v>
       </c>
-      <c r="E146" s="10" t="s">
+      <c r="E146" s="12" t="s">
         <v>149</v>
       </c>
       <c r="F146" s="11">
@@ -10313,7 +10320,7 @@
       <c r="D147" s="1">
         <v>11</v>
       </c>
-      <c r="E147" s="10" t="s">
+      <c r="E147" s="12" t="s">
         <v>150</v>
       </c>
       <c r="F147" s="11">
@@ -10333,7 +10340,7 @@
       <c r="D148" s="1">
         <v>12</v>
       </c>
-      <c r="E148" s="10" t="s">
+      <c r="E148" s="12" t="s">
         <v>151</v>
       </c>
       <c r="F148" s="11">

</xml_diff>

<commit_message>
Regex match chars that occur zero or more times
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0CBD21-B43E-4243-92D0-685C0BFDB981}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C42356-4A37-432C-9905-ABED31D50D27}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="413">
   <si>
     <t>Basic JavaScript</t>
   </si>
@@ -1256,12 +1256,36 @@
   </si>
   <si>
     <t>PassedFind More Than the First Match</t>
+  </si>
+  <si>
+    <t>PassedMatch Anything with Wildcard Period</t>
+  </si>
+  <si>
+    <t>PassedMatch Single Character with Multiple Possibilities</t>
+  </si>
+  <si>
+    <t>PassedMatch Letters of the Alphabet</t>
+  </si>
+  <si>
+    <t>PassedMatch Numbers and Letters of the Alphabet</t>
+  </si>
+  <si>
+    <t>PassedMatch Single Characters Specified</t>
+  </si>
+  <si>
+    <t>PassedMatch Characters that Occur One or More Times</t>
+  </si>
+  <si>
+    <t>PassedMatch Characters that Occur Zero or More Times</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1279,7 +1303,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1294,7 +1318,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1311,7 +1347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1332,7 +1368,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7768,8 +7809,8 @@
   <dimension ref="A1:H302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E153" sqref="E153"/>
+      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E151" sqref="E151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -7779,7 +7820,7 @@
     <col min="3" max="3" width="3.6796875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.6796875" style="1" customWidth="1"/>
     <col min="5" max="5" width="77.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.76953125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.75">
@@ -10260,8 +10301,8 @@
       <c r="D144" s="1">
         <v>8</v>
       </c>
-      <c r="E144" s="12" t="s">
-        <v>147</v>
+      <c r="E144" s="8" t="s">
+        <v>406</v>
       </c>
       <c r="F144" s="11">
         <v>43439</v>
@@ -10280,8 +10321,8 @@
       <c r="D145" s="1">
         <v>9</v>
       </c>
-      <c r="E145" s="12" t="s">
-        <v>148</v>
+      <c r="E145" s="8" t="s">
+        <v>407</v>
       </c>
       <c r="F145" s="11">
         <v>43439</v>
@@ -10300,8 +10341,8 @@
       <c r="D146" s="1">
         <v>10</v>
       </c>
-      <c r="E146" s="12" t="s">
-        <v>149</v>
+      <c r="E146" s="8" t="s">
+        <v>408</v>
       </c>
       <c r="F146" s="11">
         <v>43439</v>
@@ -10320,8 +10361,8 @@
       <c r="D147" s="1">
         <v>11</v>
       </c>
-      <c r="E147" s="12" t="s">
-        <v>150</v>
+      <c r="E147" s="8" t="s">
+        <v>409</v>
       </c>
       <c r="F147" s="11">
         <v>43439</v>
@@ -10340,8 +10381,8 @@
       <c r="D148" s="1">
         <v>12</v>
       </c>
-      <c r="E148" s="12" t="s">
-        <v>151</v>
+      <c r="E148" s="8" t="s">
+        <v>410</v>
       </c>
       <c r="F148" s="11">
         <v>43439</v>
@@ -10360,8 +10401,8 @@
       <c r="D149" s="1">
         <v>13</v>
       </c>
-      <c r="E149" s="10" t="s">
-        <v>152</v>
+      <c r="E149" s="8" t="s">
+        <v>411</v>
       </c>
       <c r="F149" s="11">
         <v>43439</v>
@@ -10380,8 +10421,8 @@
       <c r="D150" s="1">
         <v>14</v>
       </c>
-      <c r="E150" s="10" t="s">
-        <v>153</v>
+      <c r="E150" s="8" t="s">
+        <v>412</v>
       </c>
       <c r="F150" s="11">
         <v>43439</v>
@@ -10404,7 +10445,7 @@
         <v>154</v>
       </c>
       <c r="F151" s="11">
-        <v>43439</v>
+        <v>43440</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.75">
@@ -10424,7 +10465,7 @@
         <v>155</v>
       </c>
       <c r="F152" s="11">
-        <v>43439</v>
+        <v>43440</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.75">
@@ -10444,7 +10485,7 @@
         <v>156</v>
       </c>
       <c r="F153" s="11">
-        <v>43439</v>
+        <v>43440</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.75">
@@ -10460,11 +10501,11 @@
       <c r="D154" s="1">
         <v>18</v>
       </c>
-      <c r="E154" t="s">
+      <c r="E154" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="F154" s="2" t="s">
-        <v>373</v>
+      <c r="F154" s="12">
+        <v>43440</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.75">
@@ -10480,11 +10521,11 @@
       <c r="D155" s="1">
         <v>19</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E155" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="F155" s="2" t="s">
-        <v>373</v>
+      <c r="F155" s="12">
+        <v>43440</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.75">
@@ -10500,11 +10541,11 @@
       <c r="D156" s="1">
         <v>20</v>
       </c>
-      <c r="E156" t="s">
+      <c r="E156" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="F156" s="2" t="s">
-        <v>373</v>
+      <c r="F156" s="12">
+        <v>43440</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.75">
@@ -10520,11 +10561,11 @@
       <c r="D157" s="1">
         <v>21</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E157" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="F157" s="2" t="s">
-        <v>373</v>
+      <c r="F157" s="12">
+        <v>43440</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.75">
@@ -10540,11 +10581,11 @@
       <c r="D158" s="1">
         <v>22</v>
       </c>
-      <c r="E158" t="s">
+      <c r="E158" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="F158" s="2" t="s">
-        <v>373</v>
+      <c r="F158" s="12">
+        <v>43440</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.75">
@@ -10560,11 +10601,11 @@
       <c r="D159" s="1">
         <v>23</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E159" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="F159" s="2" t="s">
-        <v>373</v>
+      <c r="F159" s="12">
+        <v>43440</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.75">
@@ -10580,11 +10621,11 @@
       <c r="D160" s="1">
         <v>24</v>
       </c>
-      <c r="E160" t="s">
+      <c r="E160" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="F160" s="2" t="s">
-        <v>373</v>
+      <c r="F160" s="12">
+        <v>43440</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.75">
@@ -10600,11 +10641,11 @@
       <c r="D161" s="1">
         <v>25</v>
       </c>
-      <c r="E161" t="s">
+      <c r="E161" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="F161" s="2" t="s">
-        <v>373</v>
+      <c r="F161" s="12">
+        <v>43440</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.75">
@@ -10620,11 +10661,11 @@
       <c r="D162" s="1">
         <v>26</v>
       </c>
-      <c r="E162" t="s">
+      <c r="E162" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="F162" s="2" t="s">
-        <v>373</v>
+      <c r="F162" s="12">
+        <v>43440</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.75">
@@ -10640,11 +10681,11 @@
       <c r="D163" s="1">
         <v>27</v>
       </c>
-      <c r="E163" t="s">
+      <c r="E163" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="F163" s="2" t="s">
-        <v>373</v>
+      <c r="F163" s="12">
+        <v>43440</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.75">
@@ -10660,11 +10701,11 @@
       <c r="D164" s="1">
         <v>28</v>
       </c>
-      <c r="E164" t="s">
+      <c r="E164" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="F164" s="2" t="s">
-        <v>373</v>
+      <c r="F164" s="2">
+        <v>43441</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.75">
@@ -10680,11 +10721,11 @@
       <c r="D165" s="1">
         <v>29</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="F165" s="2" t="s">
-        <v>373</v>
+      <c r="F165" s="2">
+        <v>43441</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.75">
@@ -10700,11 +10741,11 @@
       <c r="D166" s="1">
         <v>30</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="F166" s="2" t="s">
-        <v>373</v>
+      <c r="F166" s="2">
+        <v>43441</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.75">
@@ -10720,11 +10761,11 @@
       <c r="D167" s="1">
         <v>31</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="F167" s="2" t="s">
-        <v>373</v>
+      <c r="F167" s="2">
+        <v>43441</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.75">
@@ -10740,11 +10781,11 @@
       <c r="D168" s="1">
         <v>32</v>
       </c>
-      <c r="E168" t="s">
+      <c r="E168" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="F168" s="2" t="s">
-        <v>373</v>
+      <c r="F168" s="2">
+        <v>43441</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.75">
@@ -10760,11 +10801,11 @@
       <c r="D169" s="1">
         <v>33</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="F169" s="2" t="s">
-        <v>373</v>
+      <c r="F169" s="2">
+        <v>43441</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.75">
@@ -10777,11 +10818,11 @@
       <c r="C170" s="1">
         <v>169</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="F170" s="2" t="s">
-        <v>373</v>
+      <c r="F170" s="2">
+        <v>43441</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.75">
@@ -10794,11 +10835,11 @@
       <c r="C171" s="1">
         <v>170</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="F171" s="2" t="s">
-        <v>373</v>
+      <c r="F171" s="2">
+        <v>43441</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.75">
@@ -10811,11 +10852,11 @@
       <c r="C172" s="1">
         <v>171</v>
       </c>
-      <c r="E172" t="s">
+      <c r="E172" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="F172" s="2" t="s">
-        <v>373</v>
+      <c r="F172" s="2">
+        <v>43441</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.75">
@@ -10828,11 +10869,11 @@
       <c r="C173" s="1">
         <v>172</v>
       </c>
-      <c r="E173" t="s">
+      <c r="E173" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="F173" s="2" t="s">
-        <v>373</v>
+      <c r="F173" s="2">
+        <v>43441</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.75">
@@ -10848,8 +10889,8 @@
       <c r="E174" t="s">
         <v>178</v>
       </c>
-      <c r="F174" s="2" t="s">
-        <v>373</v>
+      <c r="F174" s="15">
+        <v>43442</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.75">
@@ -10865,8 +10906,8 @@
       <c r="E175" t="s">
         <v>179</v>
       </c>
-      <c r="F175" s="2" t="s">
-        <v>373</v>
+      <c r="F175" s="2">
+        <v>43442</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.75">
@@ -10882,8 +10923,8 @@
       <c r="E176" t="s">
         <v>180</v>
       </c>
-      <c r="F176" s="2" t="s">
-        <v>373</v>
+      <c r="F176" s="2">
+        <v>43442</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.75">
@@ -10899,8 +10940,8 @@
       <c r="E177" t="s">
         <v>181</v>
       </c>
-      <c r="F177" s="2" t="s">
-        <v>373</v>
+      <c r="F177" s="2">
+        <v>43442</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.75">
@@ -10916,8 +10957,8 @@
       <c r="E178" t="s">
         <v>182</v>
       </c>
-      <c r="F178" s="2" t="s">
-        <v>373</v>
+      <c r="F178" s="2">
+        <v>43442</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.75">
@@ -10933,8 +10974,8 @@
       <c r="E179" t="s">
         <v>183</v>
       </c>
-      <c r="F179" s="2" t="s">
-        <v>373</v>
+      <c r="F179" s="2">
+        <v>43442</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.75">
@@ -10950,8 +10991,8 @@
       <c r="E180" t="s">
         <v>184</v>
       </c>
-      <c r="F180" s="2" t="s">
-        <v>373</v>
+      <c r="F180" s="2">
+        <v>43442</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.75">
@@ -10967,8 +11008,8 @@
       <c r="E181" t="s">
         <v>185</v>
       </c>
-      <c r="F181" s="2" t="s">
-        <v>373</v>
+      <c r="F181" s="2">
+        <v>43442</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.75">
@@ -10984,8 +11025,8 @@
       <c r="E182" t="s">
         <v>186</v>
       </c>
-      <c r="F182" s="2" t="s">
-        <v>373</v>
+      <c r="F182" s="2">
+        <v>43442</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.75">
@@ -11001,8 +11042,8 @@
       <c r="E183" t="s">
         <v>188</v>
       </c>
-      <c r="F183" s="2" t="s">
-        <v>373</v>
+      <c r="F183" s="2">
+        <v>43442</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.75">
@@ -11015,11 +11056,11 @@
       <c r="C184" s="1">
         <v>183</v>
       </c>
-      <c r="E184" t="s">
+      <c r="E184" s="16" t="s">
         <v>189</v>
       </c>
-      <c r="F184" s="2" t="s">
-        <v>373</v>
+      <c r="F184" s="17">
+        <v>43444</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.75">
@@ -11032,11 +11073,11 @@
       <c r="C185" s="1">
         <v>184</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="F185" s="2" t="s">
-        <v>373</v>
+      <c r="F185" s="17">
+        <v>43444</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.75">
@@ -11049,11 +11090,11 @@
       <c r="C186" s="1">
         <v>185</v>
       </c>
-      <c r="E186" t="s">
+      <c r="E186" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="F186" s="2" t="s">
-        <v>373</v>
+      <c r="F186" s="17">
+        <v>43444</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.75">
@@ -11066,11 +11107,11 @@
       <c r="C187" s="1">
         <v>186</v>
       </c>
-      <c r="E187" t="s">
+      <c r="E187" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="F187" s="2" t="s">
-        <v>373</v>
+      <c r="F187" s="17">
+        <v>43444</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.75">
@@ -11083,11 +11124,11 @@
       <c r="C188" s="1">
         <v>187</v>
       </c>
-      <c r="E188" t="s">
+      <c r="E188" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="F188" s="2" t="s">
-        <v>373</v>
+      <c r="F188" s="17">
+        <v>43444</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.75">
@@ -11100,11 +11141,11 @@
       <c r="C189" s="1">
         <v>188</v>
       </c>
-      <c r="E189" t="s">
+      <c r="E189" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="F189" s="2" t="s">
-        <v>373</v>
+      <c r="F189" s="17">
+        <v>43444</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.75">
@@ -11117,11 +11158,11 @@
       <c r="C190" s="1">
         <v>189</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="F190" s="2" t="s">
-        <v>373</v>
+      <c r="F190" s="17">
+        <v>43444</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.75">
@@ -11134,11 +11175,11 @@
       <c r="C191" s="1">
         <v>190</v>
       </c>
-      <c r="E191" t="s">
+      <c r="E191" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="F191" s="2" t="s">
-        <v>373</v>
+      <c r="F191" s="17">
+        <v>43444</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.75">
@@ -11151,11 +11192,11 @@
       <c r="C192" s="1">
         <v>191</v>
       </c>
-      <c r="E192" t="s">
+      <c r="E192" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="F192" s="2" t="s">
-        <v>373</v>
+      <c r="F192" s="17">
+        <v>43444</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.75">
@@ -11168,11 +11209,11 @@
       <c r="C193" s="1">
         <v>192</v>
       </c>
-      <c r="E193" t="s">
+      <c r="E193" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="F193" s="2" t="s">
-        <v>373</v>
+      <c r="F193" s="17">
+        <v>43444</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
Regex-Match numbers and non-numbers
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C42356-4A37-432C-9905-ABED31D50D27}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D226CDDF-E9B0-4AA1-BC40-8F1A272C7907}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="420">
   <si>
     <t>Basic JavaScript</t>
   </si>
@@ -1277,6 +1277,27 @@
   </si>
   <si>
     <t>PassedMatch Characters that Occur Zero or More Times</t>
+  </si>
+  <si>
+    <t>PassedFind Characters with Lazy Matching</t>
+  </si>
+  <si>
+    <t>PassedFind One or More Criminals in a Hunt</t>
+  </si>
+  <si>
+    <t>PassedMatch Beginning String Patterns</t>
+  </si>
+  <si>
+    <t>PassedMatch Ending String Patterns</t>
+  </si>
+  <si>
+    <t>PassedMatch All Letters and Numbers</t>
+  </si>
+  <si>
+    <t>PassedMatch Everything But Letters and Numbers</t>
+  </si>
+  <si>
+    <t>PassedMatch All Numbers</t>
   </si>
 </sst>
 </file>
@@ -1284,7 +1305,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1366,14 +1387,14 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7809,8 +7830,8 @@
   <dimension ref="A1:H302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E151" sqref="E151"/>
+      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F159" sqref="F159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -10304,7 +10325,7 @@
       <c r="E144" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="F144" s="11">
+      <c r="F144" s="10">
         <v>43439</v>
       </c>
     </row>
@@ -10324,7 +10345,7 @@
       <c r="E145" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="F145" s="11">
+      <c r="F145" s="10">
         <v>43439</v>
       </c>
     </row>
@@ -10344,7 +10365,7 @@
       <c r="E146" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="F146" s="11">
+      <c r="F146" s="10">
         <v>43439</v>
       </c>
     </row>
@@ -10364,7 +10385,7 @@
       <c r="E147" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="F147" s="11">
+      <c r="F147" s="10">
         <v>43439</v>
       </c>
     </row>
@@ -10384,7 +10405,7 @@
       <c r="E148" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="F148" s="11">
+      <c r="F148" s="10">
         <v>43439</v>
       </c>
     </row>
@@ -10404,7 +10425,7 @@
       <c r="E149" s="8" t="s">
         <v>411</v>
       </c>
-      <c r="F149" s="11">
+      <c r="F149" s="10">
         <v>43439</v>
       </c>
     </row>
@@ -10424,7 +10445,7 @@
       <c r="E150" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="F150" s="11">
+      <c r="F150" s="10">
         <v>43439</v>
       </c>
     </row>
@@ -10441,11 +10462,11 @@
       <c r="D151" s="1">
         <v>15</v>
       </c>
-      <c r="E151" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="F151" s="11">
-        <v>43440</v>
+      <c r="E151" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="F151" s="10">
+        <v>43444</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.75">
@@ -10461,11 +10482,11 @@
       <c r="D152" s="1">
         <v>16</v>
       </c>
-      <c r="E152" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="F152" s="11">
-        <v>43440</v>
+      <c r="E152" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="F152" s="10">
+        <v>43444</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.75">
@@ -10481,11 +10502,11 @@
       <c r="D153" s="1">
         <v>17</v>
       </c>
-      <c r="E153" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="F153" s="11">
-        <v>43440</v>
+      <c r="E153" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="F153" s="10">
+        <v>43444</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.75">
@@ -10501,11 +10522,11 @@
       <c r="D154" s="1">
         <v>18</v>
       </c>
-      <c r="E154" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="F154" s="12">
-        <v>43440</v>
+      <c r="E154" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="F154" s="10">
+        <v>43444</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.75">
@@ -10521,11 +10542,11 @@
       <c r="D155" s="1">
         <v>19</v>
       </c>
-      <c r="E155" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="F155" s="12">
-        <v>43440</v>
+      <c r="E155" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="F155" s="10">
+        <v>43444</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.75">
@@ -10541,11 +10562,11 @@
       <c r="D156" s="1">
         <v>20</v>
       </c>
-      <c r="E156" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="F156" s="12">
-        <v>43440</v>
+      <c r="E156" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="F156" s="10">
+        <v>43444</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.75">
@@ -10561,11 +10582,11 @@
       <c r="D157" s="1">
         <v>21</v>
       </c>
-      <c r="E157" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="F157" s="12">
-        <v>43440</v>
+      <c r="E157" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="F157" s="10">
+        <v>43444</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.75">
@@ -10581,11 +10602,11 @@
       <c r="D158" s="1">
         <v>22</v>
       </c>
-      <c r="E158" s="13" t="s">
+      <c r="E158" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="F158" s="12">
-        <v>43440</v>
+      <c r="F158" s="11">
+        <v>43445</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.75">
@@ -10601,11 +10622,11 @@
       <c r="D159" s="1">
         <v>23</v>
       </c>
-      <c r="E159" s="13" t="s">
+      <c r="E159" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="F159" s="12">
-        <v>43440</v>
+      <c r="F159" s="11">
+        <v>43445</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.75">
@@ -10621,11 +10642,11 @@
       <c r="D160" s="1">
         <v>24</v>
       </c>
-      <c r="E160" s="13" t="s">
+      <c r="E160" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="F160" s="12">
-        <v>43440</v>
+      <c r="F160" s="11">
+        <v>43445</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.75">
@@ -10641,11 +10662,11 @@
       <c r="D161" s="1">
         <v>25</v>
       </c>
-      <c r="E161" s="13" t="s">
+      <c r="E161" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="F161" s="12">
-        <v>43440</v>
+      <c r="F161" s="11">
+        <v>43445</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.75">
@@ -10661,11 +10682,11 @@
       <c r="D162" s="1">
         <v>26</v>
       </c>
-      <c r="E162" s="13" t="s">
+      <c r="E162" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="F162" s="12">
-        <v>43440</v>
+      <c r="F162" s="11">
+        <v>43445</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.75">
@@ -10681,11 +10702,11 @@
       <c r="D163" s="1">
         <v>27</v>
       </c>
-      <c r="E163" s="13" t="s">
+      <c r="E163" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="F163" s="12">
-        <v>43440</v>
+      <c r="F163" s="11">
+        <v>43445</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.75">
@@ -10701,11 +10722,11 @@
       <c r="D164" s="1">
         <v>28</v>
       </c>
-      <c r="E164" s="14" t="s">
+      <c r="E164" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="F164" s="2">
-        <v>43441</v>
+      <c r="F164" s="11">
+        <v>43445</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.75">
@@ -10721,11 +10742,11 @@
       <c r="D165" s="1">
         <v>29</v>
       </c>
-      <c r="E165" s="14" t="s">
+      <c r="E165" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="F165" s="2">
-        <v>43441</v>
+      <c r="F165" s="11">
+        <v>43445</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.75">
@@ -10741,11 +10762,11 @@
       <c r="D166" s="1">
         <v>30</v>
       </c>
-      <c r="E166" s="14" t="s">
+      <c r="E166" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="F166" s="2">
-        <v>43441</v>
+      <c r="F166" s="11">
+        <v>43445</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.75">
@@ -10761,11 +10782,11 @@
       <c r="D167" s="1">
         <v>31</v>
       </c>
-      <c r="E167" s="14" t="s">
+      <c r="E167" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="F167" s="2">
-        <v>43441</v>
+      <c r="F167" s="11">
+        <v>43445</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.75">
@@ -10781,11 +10802,11 @@
       <c r="D168" s="1">
         <v>32</v>
       </c>
-      <c r="E168" s="14" t="s">
+      <c r="E168" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="F168" s="2">
-        <v>43441</v>
+      <c r="F168" s="11">
+        <v>43445</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.75">
@@ -10801,11 +10822,11 @@
       <c r="D169" s="1">
         <v>33</v>
       </c>
-      <c r="E169" s="14" t="s">
+      <c r="E169" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="F169" s="2">
-        <v>43441</v>
+      <c r="F169" s="11">
+        <v>43445</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.75">
@@ -10818,7 +10839,7 @@
       <c r="C170" s="1">
         <v>169</v>
       </c>
-      <c r="E170" s="14" t="s">
+      <c r="E170" s="12" t="s">
         <v>174</v>
       </c>
       <c r="F170" s="2">
@@ -10835,7 +10856,7 @@
       <c r="C171" s="1">
         <v>170</v>
       </c>
-      <c r="E171" s="14" t="s">
+      <c r="E171" s="12" t="s">
         <v>175</v>
       </c>
       <c r="F171" s="2">
@@ -10852,7 +10873,7 @@
       <c r="C172" s="1">
         <v>171</v>
       </c>
-      <c r="E172" s="14" t="s">
+      <c r="E172" s="12" t="s">
         <v>176</v>
       </c>
       <c r="F172" s="2">
@@ -10869,7 +10890,7 @@
       <c r="C173" s="1">
         <v>172</v>
       </c>
-      <c r="E173" s="14" t="s">
+      <c r="E173" s="12" t="s">
         <v>177</v>
       </c>
       <c r="F173" s="2">
@@ -10889,7 +10910,7 @@
       <c r="E174" t="s">
         <v>178</v>
       </c>
-      <c r="F174" s="15">
+      <c r="F174" s="13">
         <v>43442</v>
       </c>
     </row>
@@ -11056,10 +11077,10 @@
       <c r="C184" s="1">
         <v>183</v>
       </c>
-      <c r="E184" s="16" t="s">
+      <c r="E184" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="F184" s="17">
+      <c r="F184" s="15">
         <v>43444</v>
       </c>
     </row>
@@ -11073,10 +11094,10 @@
       <c r="C185" s="1">
         <v>184</v>
       </c>
-      <c r="E185" s="16" t="s">
+      <c r="E185" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="F185" s="17">
+      <c r="F185" s="15">
         <v>43444</v>
       </c>
     </row>
@@ -11090,10 +11111,10 @@
       <c r="C186" s="1">
         <v>185</v>
       </c>
-      <c r="E186" s="16" t="s">
+      <c r="E186" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="F186" s="17">
+      <c r="F186" s="15">
         <v>43444</v>
       </c>
     </row>
@@ -11107,10 +11128,10 @@
       <c r="C187" s="1">
         <v>186</v>
       </c>
-      <c r="E187" s="16" t="s">
+      <c r="E187" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="F187" s="17">
+      <c r="F187" s="15">
         <v>43444</v>
       </c>
     </row>
@@ -11124,10 +11145,10 @@
       <c r="C188" s="1">
         <v>187</v>
       </c>
-      <c r="E188" s="16" t="s">
+      <c r="E188" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="F188" s="17">
+      <c r="F188" s="15">
         <v>43444</v>
       </c>
     </row>
@@ -11141,10 +11162,10 @@
       <c r="C189" s="1">
         <v>188</v>
       </c>
-      <c r="E189" s="16" t="s">
+      <c r="E189" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="F189" s="17">
+      <c r="F189" s="15">
         <v>43444</v>
       </c>
     </row>
@@ -11158,10 +11179,10 @@
       <c r="C190" s="1">
         <v>189</v>
       </c>
-      <c r="E190" s="16" t="s">
+      <c r="E190" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="F190" s="17">
+      <c r="F190" s="15">
         <v>43444</v>
       </c>
     </row>
@@ -11175,10 +11196,10 @@
       <c r="C191" s="1">
         <v>190</v>
       </c>
-      <c r="E191" s="16" t="s">
+      <c r="E191" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="F191" s="17">
+      <c r="F191" s="15">
         <v>43444</v>
       </c>
     </row>
@@ -11192,10 +11213,10 @@
       <c r="C192" s="1">
         <v>191</v>
       </c>
-      <c r="E192" s="16" t="s">
+      <c r="E192" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="F192" s="17">
+      <c r="F192" s="15">
         <v>43444</v>
       </c>
     </row>
@@ -11209,10 +11230,10 @@
       <c r="C193" s="1">
         <v>192</v>
       </c>
-      <c r="E193" s="16" t="s">
+      <c r="E193" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="F193" s="17">
+      <c r="F193" s="15">
         <v>43444</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Regex - Exact number of matches
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D226CDDF-E9B0-4AA1-BC40-8F1A272C7907}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B990D60-1683-43E9-BD9B-D2DE5A7A69EA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
@@ -1304,9 +1304,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1368,7 +1365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1390,11 +1387,10 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7830,8 +7826,8 @@
   <dimension ref="A1:H302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F159" sqref="F159"/>
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E174" sqref="E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -10722,7 +10718,7 @@
       <c r="D164" s="1">
         <v>28</v>
       </c>
-      <c r="E164" s="17" t="s">
+      <c r="E164" s="16" t="s">
         <v>167</v>
       </c>
       <c r="F164" s="11">
@@ -10742,11 +10738,11 @@
       <c r="D165" s="1">
         <v>29</v>
       </c>
-      <c r="E165" s="17" t="s">
+      <c r="E165" s="15" t="s">
         <v>168</v>
       </c>
       <c r="F165" s="11">
-        <v>43445</v>
+        <v>43446</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.75">
@@ -10762,11 +10758,11 @@
       <c r="D166" s="1">
         <v>30</v>
       </c>
-      <c r="E166" s="17" t="s">
+      <c r="E166" s="15" t="s">
         <v>169</v>
       </c>
       <c r="F166" s="11">
-        <v>43445</v>
+        <v>43446</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.75">
@@ -10782,11 +10778,11 @@
       <c r="D167" s="1">
         <v>31</v>
       </c>
-      <c r="E167" s="17" t="s">
+      <c r="E167" s="15" t="s">
         <v>170</v>
       </c>
       <c r="F167" s="11">
-        <v>43445</v>
+        <v>43446</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.75">
@@ -10802,11 +10798,11 @@
       <c r="D168" s="1">
         <v>32</v>
       </c>
-      <c r="E168" s="17" t="s">
+      <c r="E168" s="15" t="s">
         <v>171</v>
       </c>
       <c r="F168" s="11">
-        <v>43445</v>
+        <v>43446</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.75">
@@ -10822,11 +10818,11 @@
       <c r="D169" s="1">
         <v>33</v>
       </c>
-      <c r="E169" s="17" t="s">
+      <c r="E169" s="15" t="s">
         <v>172</v>
       </c>
       <c r="F169" s="11">
-        <v>43445</v>
+        <v>43446</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.75">
@@ -10842,8 +10838,8 @@
       <c r="E170" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="F170" s="2">
-        <v>43441</v>
+      <c r="F170" s="11">
+        <v>43446</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.75">
@@ -10859,8 +10855,8 @@
       <c r="E171" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="F171" s="2">
-        <v>43441</v>
+      <c r="F171" s="11">
+        <v>43446</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.75">
@@ -10876,8 +10872,8 @@
       <c r="E172" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="F172" s="2">
-        <v>43441</v>
+      <c r="F172" s="11">
+        <v>43446</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.75">
@@ -10893,8 +10889,8 @@
       <c r="E173" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="F173" s="2">
-        <v>43441</v>
+      <c r="F173" s="11">
+        <v>43446</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.75">
@@ -10907,11 +10903,11 @@
       <c r="C174" s="1">
         <v>173</v>
       </c>
-      <c r="E174" t="s">
+      <c r="E174" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F174" s="13">
-        <v>43442</v>
+      <c r="F174" s="11">
+        <v>43446</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.75">
@@ -11077,10 +11073,10 @@
       <c r="C184" s="1">
         <v>183</v>
       </c>
-      <c r="E184" s="14" t="s">
+      <c r="E184" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="F184" s="15">
+      <c r="F184" s="14">
         <v>43444</v>
       </c>
     </row>
@@ -11094,10 +11090,10 @@
       <c r="C185" s="1">
         <v>184</v>
       </c>
-      <c r="E185" s="14" t="s">
+      <c r="E185" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="F185" s="15">
+      <c r="F185" s="14">
         <v>43444</v>
       </c>
     </row>
@@ -11111,10 +11107,10 @@
       <c r="C186" s="1">
         <v>185</v>
       </c>
-      <c r="E186" s="14" t="s">
+      <c r="E186" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="F186" s="15">
+      <c r="F186" s="14">
         <v>43444</v>
       </c>
     </row>
@@ -11128,10 +11124,10 @@
       <c r="C187" s="1">
         <v>186</v>
       </c>
-      <c r="E187" s="14" t="s">
+      <c r="E187" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="F187" s="15">
+      <c r="F187" s="14">
         <v>43444</v>
       </c>
     </row>
@@ -11145,10 +11141,10 @@
       <c r="C188" s="1">
         <v>187</v>
       </c>
-      <c r="E188" s="14" t="s">
+      <c r="E188" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="F188" s="15">
+      <c r="F188" s="14">
         <v>43444</v>
       </c>
     </row>
@@ -11162,10 +11158,10 @@
       <c r="C189" s="1">
         <v>188</v>
       </c>
-      <c r="E189" s="14" t="s">
+      <c r="E189" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="F189" s="15">
+      <c r="F189" s="14">
         <v>43444</v>
       </c>
     </row>
@@ -11179,10 +11175,10 @@
       <c r="C190" s="1">
         <v>189</v>
       </c>
-      <c r="E190" s="14" t="s">
+      <c r="E190" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="F190" s="15">
+      <c r="F190" s="14">
         <v>43444</v>
       </c>
     </row>
@@ -11196,10 +11192,10 @@
       <c r="C191" s="1">
         <v>190</v>
       </c>
-      <c r="E191" s="14" t="s">
+      <c r="E191" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="F191" s="15">
+      <c r="F191" s="14">
         <v>43444</v>
       </c>
     </row>
@@ -11213,10 +11209,10 @@
       <c r="C192" s="1">
         <v>191</v>
       </c>
-      <c r="E192" s="14" t="s">
+      <c r="E192" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="F192" s="15">
+      <c r="F192" s="14">
         <v>43444</v>
       </c>
     </row>
@@ -11230,10 +11226,10 @@
       <c r="C193" s="1">
         <v>192</v>
       </c>
-      <c r="E193" s="14" t="s">
+      <c r="E193" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="F193" s="15">
+      <c r="F193" s="14">
         <v>43444</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Key-Value Pairs to JavaScript Objects
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BCB5F1-BF0E-49DD-8B8B-4038144BF829}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D1CAB6-E299-4B20-9EEF-EA090EAB2FD3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="455">
   <si>
     <t>Basic JavaScript</t>
   </si>
@@ -1382,6 +1382,27 @@
   </si>
   <si>
     <t>PassedRemove Items Using splice()</t>
+  </si>
+  <si>
+    <t>PassedAdd Items Using splice()</t>
+  </si>
+  <si>
+    <t>PassedCopy Array Items Using slice()</t>
+  </si>
+  <si>
+    <t>PassedCopy an Array with the Spread Operator</t>
+  </si>
+  <si>
+    <t>PassedCombine Arrays with the Spread Operator</t>
+  </si>
+  <si>
+    <t>PassedCheck For The Presence of an Element With indexOf()</t>
+  </si>
+  <si>
+    <t>PassedIterate Through All an Array's Items Using For Loops</t>
+  </si>
+  <si>
+    <t>PassedCreate complex multi-dimensional arrays</t>
   </si>
 </sst>
 </file>
@@ -7902,10 +7923,10 @@
   <dimension ref="A1:H302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B287" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B288" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F295" sqref="F295:F299"/>
+      <selection pane="bottomRight" activeCell="E296" sqref="E296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -11296,8 +11317,8 @@
       <c r="D189" s="1">
         <v>7</v>
       </c>
-      <c r="E189" s="13" t="s">
-        <v>194</v>
+      <c r="E189" s="14" t="s">
+        <v>448</v>
       </c>
       <c r="F189" s="12">
         <v>43461</v>
@@ -11316,8 +11337,8 @@
       <c r="D190" s="1">
         <v>8</v>
       </c>
-      <c r="E190" s="13" t="s">
-        <v>195</v>
+      <c r="E190" s="14" t="s">
+        <v>449</v>
       </c>
       <c r="F190" s="12">
         <v>43461</v>
@@ -11336,8 +11357,8 @@
       <c r="D191" s="1">
         <v>9</v>
       </c>
-      <c r="E191" s="13" t="s">
-        <v>196</v>
+      <c r="E191" s="14" t="s">
+        <v>450</v>
       </c>
       <c r="F191" s="12">
         <v>43461</v>
@@ -11356,8 +11377,8 @@
       <c r="D192" s="1">
         <v>10</v>
       </c>
-      <c r="E192" s="13" t="s">
-        <v>197</v>
+      <c r="E192" s="14" t="s">
+        <v>451</v>
       </c>
       <c r="F192" s="12">
         <v>43461</v>
@@ -11376,8 +11397,8 @@
       <c r="D193" s="1">
         <v>11</v>
       </c>
-      <c r="E193" s="13" t="s">
-        <v>198</v>
+      <c r="E193" s="14" t="s">
+        <v>452</v>
       </c>
       <c r="F193" s="12">
         <v>43461</v>
@@ -11396,11 +11417,11 @@
       <c r="D194" s="1">
         <v>12</v>
       </c>
-      <c r="E194" s="13" t="s">
-        <v>199</v>
+      <c r="E194" s="14" t="s">
+        <v>453</v>
       </c>
       <c r="F194" s="12">
-        <v>43462</v>
+        <v>43468</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.75">
@@ -11416,11 +11437,11 @@
       <c r="D195" s="1">
         <v>13</v>
       </c>
-      <c r="E195" s="13" t="s">
-        <v>200</v>
+      <c r="E195" s="14" t="s">
+        <v>454</v>
       </c>
       <c r="F195" s="12">
-        <v>43462</v>
+        <v>43468</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.75">
@@ -11440,7 +11461,7 @@
         <v>201</v>
       </c>
       <c r="F196" s="12">
-        <v>43462</v>
+        <v>43469</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.75">
@@ -11460,7 +11481,7 @@
         <v>202</v>
       </c>
       <c r="F197" s="12">
-        <v>43462</v>
+        <v>43469</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.75">
@@ -11480,7 +11501,7 @@
         <v>203</v>
       </c>
       <c r="F198" s="12">
-        <v>43462</v>
+        <v>43469</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.75">
@@ -11500,7 +11521,7 @@
         <v>204</v>
       </c>
       <c r="F199" s="12">
-        <v>43462</v>
+        <v>43469</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.75">
@@ -11520,7 +11541,7 @@
         <v>205</v>
       </c>
       <c r="F200" s="12">
-        <v>43462</v>
+        <v>43469</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.75">
@@ -11540,7 +11561,7 @@
         <v>206</v>
       </c>
       <c r="F201" s="12">
-        <v>43462</v>
+        <v>43469</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.75">
@@ -11560,7 +11581,7 @@
         <v>207</v>
       </c>
       <c r="F202" s="12">
-        <v>43462</v>
+        <v>43469</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.75">
@@ -11580,7 +11601,7 @@
         <v>208</v>
       </c>
       <c r="F203" s="12">
-        <v>43462</v>
+        <v>43469</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.75">
@@ -11596,8 +11617,8 @@
       <c r="E204" t="s">
         <v>210</v>
       </c>
-      <c r="F204" s="2">
-        <v>43463</v>
+      <c r="F204" s="12">
+        <v>43469</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.75">
@@ -11613,8 +11634,8 @@
       <c r="E205" t="s">
         <v>211</v>
       </c>
-      <c r="F205" s="2">
-        <v>43463</v>
+      <c r="F205" s="12">
+        <v>43469</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.75">
@@ -11631,7 +11652,7 @@
         <v>212</v>
       </c>
       <c r="F206" s="2">
-        <v>43463</v>
+        <v>43470</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.75">
@@ -11648,7 +11669,7 @@
         <v>213</v>
       </c>
       <c r="F207" s="2">
-        <v>43463</v>
+        <v>43470</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.75">
@@ -11665,7 +11686,7 @@
         <v>214</v>
       </c>
       <c r="F208" s="2">
-        <v>43463</v>
+        <v>43470</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.75">
@@ -11682,7 +11703,7 @@
         <v>215</v>
       </c>
       <c r="F209" s="2">
-        <v>43463</v>
+        <v>43470</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.75">
@@ -11699,7 +11720,7 @@
         <v>216</v>
       </c>
       <c r="F210" s="2">
-        <v>43463</v>
+        <v>43470</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.75">
@@ -11716,7 +11737,7 @@
         <v>217</v>
       </c>
       <c r="F211" s="2">
-        <v>43463</v>
+        <v>43470</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.75">
@@ -11733,7 +11754,7 @@
         <v>218</v>
       </c>
       <c r="F212" s="2">
-        <v>43463</v>
+        <v>43470</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.75">
@@ -11750,7 +11771,7 @@
         <v>219</v>
       </c>
       <c r="F213" s="2">
-        <v>43463</v>
+        <v>43470</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.75">
@@ -11767,7 +11788,7 @@
         <v>220</v>
       </c>
       <c r="F214" s="2">
-        <v>43466</v>
+        <v>43470</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.75">
@@ -11784,7 +11805,7 @@
         <v>221</v>
       </c>
       <c r="F215" s="2">
-        <v>43466</v>
+        <v>43470</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.75">
@@ -11801,7 +11822,7 @@
         <v>222</v>
       </c>
       <c r="F216" s="2">
-        <v>43466</v>
+        <v>43471</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.75">
@@ -11818,7 +11839,7 @@
         <v>223</v>
       </c>
       <c r="F217" s="2">
-        <v>43466</v>
+        <v>43471</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.75">
@@ -11835,7 +11856,7 @@
         <v>224</v>
       </c>
       <c r="F218" s="2">
-        <v>43466</v>
+        <v>43471</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.75">
@@ -11852,7 +11873,7 @@
         <v>225</v>
       </c>
       <c r="F219" s="2">
-        <v>43466</v>
+        <v>43471</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.75">
@@ -11869,7 +11890,7 @@
         <v>226</v>
       </c>
       <c r="F220" s="2">
-        <v>43466</v>
+        <v>43471</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.75">
@@ -11886,7 +11907,7 @@
         <v>228</v>
       </c>
       <c r="F221" s="2">
-        <v>43466</v>
+        <v>43471</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.75">
@@ -11903,7 +11924,7 @@
         <v>229</v>
       </c>
       <c r="F222" s="2">
-        <v>43466</v>
+        <v>43471</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.75">
@@ -11920,7 +11941,7 @@
         <v>230</v>
       </c>
       <c r="F223" s="2">
-        <v>43466</v>
+        <v>43471</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.75">
@@ -11937,7 +11958,7 @@
         <v>231</v>
       </c>
       <c r="F224" s="2">
-        <v>43467</v>
+        <v>43471</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.75">
@@ -11954,7 +11975,7 @@
         <v>232</v>
       </c>
       <c r="F225" s="2">
-        <v>43467</v>
+        <v>43471</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.75">
@@ -11971,7 +11992,7 @@
         <v>233</v>
       </c>
       <c r="F226" s="2">
-        <v>43467</v>
+        <v>43472</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.75">
@@ -11988,7 +12009,7 @@
         <v>234</v>
       </c>
       <c r="F227" s="2">
-        <v>43467</v>
+        <v>43472</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.75">
@@ -12005,7 +12026,7 @@
         <v>235</v>
       </c>
       <c r="F228" s="2">
-        <v>43467</v>
+        <v>43472</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.75">
@@ -12022,7 +12043,7 @@
         <v>236</v>
       </c>
       <c r="F229" s="2">
-        <v>43467</v>
+        <v>43472</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.75">
@@ -12039,7 +12060,7 @@
         <v>237</v>
       </c>
       <c r="F230" s="2">
-        <v>43467</v>
+        <v>43472</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.75">
@@ -12056,7 +12077,7 @@
         <v>238</v>
       </c>
       <c r="F231" s="2">
-        <v>43467</v>
+        <v>43472</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.75">
@@ -12073,7 +12094,7 @@
         <v>239</v>
       </c>
       <c r="F232" s="2">
-        <v>43467</v>
+        <v>43472</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.75">
@@ -12090,7 +12111,7 @@
         <v>240</v>
       </c>
       <c r="F233" s="2">
-        <v>43467</v>
+        <v>43472</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.75">
@@ -12107,7 +12128,7 @@
         <v>241</v>
       </c>
       <c r="F234" s="2">
-        <v>43468</v>
+        <v>43472</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.75">
@@ -12124,7 +12145,7 @@
         <v>242</v>
       </c>
       <c r="F235" s="2">
-        <v>43468</v>
+        <v>43472</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.75">
@@ -12141,7 +12162,7 @@
         <v>243</v>
       </c>
       <c r="F236" s="2">
-        <v>43468</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.75">
@@ -12158,7 +12179,7 @@
         <v>244</v>
       </c>
       <c r="F237" s="2">
-        <v>43468</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.75">
@@ -12175,7 +12196,7 @@
         <v>245</v>
       </c>
       <c r="F238" s="2">
-        <v>43468</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.75">
@@ -12192,7 +12213,7 @@
         <v>246</v>
       </c>
       <c r="F239" s="2">
-        <v>43468</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.75">
@@ -12209,7 +12230,7 @@
         <v>247</v>
       </c>
       <c r="F240" s="2">
-        <v>43468</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.75">
@@ -12226,7 +12247,7 @@
         <v>248</v>
       </c>
       <c r="F241" s="2">
-        <v>43468</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.75">
@@ -12243,7 +12264,7 @@
         <v>249</v>
       </c>
       <c r="F242" s="2">
-        <v>43468</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.75">
@@ -12260,7 +12281,7 @@
         <v>250</v>
       </c>
       <c r="F243" s="2">
-        <v>43468</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.75">
@@ -12277,7 +12298,7 @@
         <v>251</v>
       </c>
       <c r="F244" s="2">
-        <v>43469</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.75">
@@ -12294,7 +12315,7 @@
         <v>252</v>
       </c>
       <c r="F245" s="2">
-        <v>43469</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.75">
@@ -12311,7 +12332,7 @@
         <v>253</v>
       </c>
       <c r="F246" s="2">
-        <v>43469</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.75">
@@ -12328,7 +12349,7 @@
         <v>254</v>
       </c>
       <c r="F247" s="2">
-        <v>43469</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.75">
@@ -12345,7 +12366,7 @@
         <v>256</v>
       </c>
       <c r="F248" s="2">
-        <v>43469</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.75">
@@ -12362,7 +12383,7 @@
         <v>257</v>
       </c>
       <c r="F249" s="2">
-        <v>43469</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.75">
@@ -12379,7 +12400,7 @@
         <v>258</v>
       </c>
       <c r="F250" s="2">
-        <v>43469</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.75">
@@ -12396,7 +12417,7 @@
         <v>259</v>
       </c>
       <c r="F251" s="2">
-        <v>43469</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.75">
@@ -12413,7 +12434,7 @@
         <v>260</v>
       </c>
       <c r="F252" s="2">
-        <v>43469</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.75">
@@ -12430,7 +12451,7 @@
         <v>261</v>
       </c>
       <c r="F253" s="2">
-        <v>43469</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.75">
@@ -12447,7 +12468,7 @@
         <v>262</v>
       </c>
       <c r="F254" s="2">
-        <v>43470</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.75">
@@ -12464,7 +12485,7 @@
         <v>263</v>
       </c>
       <c r="F255" s="2">
-        <v>43470</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.75">
@@ -12481,7 +12502,7 @@
         <v>264</v>
       </c>
       <c r="F256" s="2">
-        <v>43470</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.75">
@@ -12498,7 +12519,7 @@
         <v>265</v>
       </c>
       <c r="F257" s="2">
-        <v>43470</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.75">
@@ -12515,7 +12536,7 @@
         <v>266</v>
       </c>
       <c r="F258" s="2">
-        <v>43470</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.75">
@@ -12532,7 +12553,7 @@
         <v>267</v>
       </c>
       <c r="F259" s="2">
-        <v>43470</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.75">
@@ -12549,7 +12570,7 @@
         <v>268</v>
       </c>
       <c r="F260" s="2">
-        <v>43470</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.75">
@@ -12566,7 +12587,7 @@
         <v>269</v>
       </c>
       <c r="F261" s="2">
-        <v>43470</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.75">
@@ -12583,7 +12604,7 @@
         <v>270</v>
       </c>
       <c r="F262" s="2">
-        <v>43470</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.75">
@@ -12600,7 +12621,7 @@
         <v>271</v>
       </c>
       <c r="F263" s="2">
-        <v>43470</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.75">
@@ -12617,7 +12638,7 @@
         <v>272</v>
       </c>
       <c r="F264" s="2">
-        <v>43471</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.75">
@@ -12634,7 +12655,7 @@
         <v>273</v>
       </c>
       <c r="F265" s="2">
-        <v>43471</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.75">
@@ -12651,7 +12672,7 @@
         <v>274</v>
       </c>
       <c r="F266" s="2">
-        <v>43471</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.75">
@@ -12668,7 +12689,7 @@
         <v>275</v>
       </c>
       <c r="F267" s="2">
-        <v>43471</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.75">
@@ -12685,7 +12706,7 @@
         <v>276</v>
       </c>
       <c r="F268" s="2">
-        <v>43471</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.75">
@@ -12702,7 +12723,7 @@
         <v>277</v>
       </c>
       <c r="F269" s="2">
-        <v>43471</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.75">
@@ -12719,7 +12740,7 @@
         <v>278</v>
       </c>
       <c r="F270" s="2">
-        <v>43471</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.75">
@@ -12736,7 +12757,7 @@
         <v>279</v>
       </c>
       <c r="F271" s="2">
-        <v>43471</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.75">
@@ -12753,7 +12774,7 @@
         <v>281</v>
       </c>
       <c r="F272" s="2">
-        <v>43471</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.75">
@@ -12770,7 +12791,7 @@
         <v>282</v>
       </c>
       <c r="F273" s="2">
-        <v>43471</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.75">
@@ -12787,7 +12808,7 @@
         <v>283</v>
       </c>
       <c r="F274" s="2">
-        <v>43472</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.75">
@@ -12804,7 +12825,7 @@
         <v>284</v>
       </c>
       <c r="F275" s="2">
-        <v>43472</v>
+        <v>43476</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.75">
@@ -12821,7 +12842,7 @@
         <v>285</v>
       </c>
       <c r="F276" s="2">
-        <v>43472</v>
+        <v>43477</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.75">
@@ -12838,7 +12859,7 @@
         <v>286</v>
       </c>
       <c r="F277" s="2">
-        <v>43472</v>
+        <v>43477</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.75">
@@ -12855,7 +12876,7 @@
         <v>287</v>
       </c>
       <c r="F278" s="2">
-        <v>43472</v>
+        <v>43477</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.75">
@@ -12872,7 +12893,7 @@
         <v>288</v>
       </c>
       <c r="F279" s="2">
-        <v>43472</v>
+        <v>43477</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.75">
@@ -12889,7 +12910,7 @@
         <v>289</v>
       </c>
       <c r="F280" s="2">
-        <v>43472</v>
+        <v>43477</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.75">
@@ -12906,7 +12927,7 @@
         <v>290</v>
       </c>
       <c r="F281" s="2">
-        <v>43472</v>
+        <v>43477</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.75">
@@ -12923,7 +12944,7 @@
         <v>291</v>
       </c>
       <c r="F282" s="2">
-        <v>43472</v>
+        <v>43477</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.75">
@@ -12940,7 +12961,7 @@
         <v>292</v>
       </c>
       <c r="F283" s="2">
-        <v>43472</v>
+        <v>43477</v>
       </c>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.75">
@@ -12957,7 +12978,7 @@
         <v>293</v>
       </c>
       <c r="F284" s="2">
-        <v>43473</v>
+        <v>43477</v>
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.75">
@@ -12974,7 +12995,7 @@
         <v>294</v>
       </c>
       <c r="F285" s="2">
-        <v>43473</v>
+        <v>43477</v>
       </c>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.75">
@@ -12991,7 +13012,7 @@
         <v>295</v>
       </c>
       <c r="F286" s="2">
-        <v>43473</v>
+        <v>43478</v>
       </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.75">
@@ -13008,7 +13029,7 @@
         <v>296</v>
       </c>
       <c r="F287" s="2">
-        <v>43473</v>
+        <v>43478</v>
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.75">
@@ -13025,7 +13046,7 @@
         <v>297</v>
       </c>
       <c r="F288" s="2">
-        <v>43473</v>
+        <v>43478</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.75">
@@ -13042,7 +13063,7 @@
         <v>298</v>
       </c>
       <c r="F289" s="2">
-        <v>43473</v>
+        <v>43478</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.75">
@@ -13059,7 +13080,7 @@
         <v>299</v>
       </c>
       <c r="F290" s="2">
-        <v>43473</v>
+        <v>43478</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.75">
@@ -13076,7 +13097,7 @@
         <v>300</v>
       </c>
       <c r="F291" s="2">
-        <v>43473</v>
+        <v>43478</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.75">
@@ -13093,7 +13114,7 @@
         <v>301</v>
       </c>
       <c r="F292" s="2">
-        <v>43473</v>
+        <v>43478</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.75">
@@ -13110,7 +13131,7 @@
         <v>302</v>
       </c>
       <c r="F293" s="2">
-        <v>43473</v>
+        <v>43478</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.75">
@@ -13127,7 +13148,7 @@
         <v>304</v>
       </c>
       <c r="F294" s="2">
-        <v>43474</v>
+        <v>43478</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.75">
@@ -13144,7 +13165,7 @@
         <v>305</v>
       </c>
       <c r="F295" s="2">
-        <v>43474</v>
+        <v>43478</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.75">
@@ -13161,7 +13182,7 @@
         <v>306</v>
       </c>
       <c r="F296" s="2">
-        <v>43474</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.75">
@@ -13178,7 +13199,7 @@
         <v>307</v>
       </c>
       <c r="F297" s="2">
-        <v>43474</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.75">
@@ -13195,7 +13216,7 @@
         <v>308</v>
       </c>
       <c r="F298" s="2">
-        <v>43474</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.75">
@@ -13212,7 +13233,7 @@
         <v>309</v>
       </c>
       <c r="F299" s="2">
-        <v>43474</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.75">

</xml_diff>

<commit_message>
JS Udemy create projects Operators
</commit_message>
<xml_diff>
--- a/FreeCodeCamp.xlsx
+++ b/FreeCodeCamp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faith\EFMCODER\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5AFD7C-0273-4A45-B5D1-83580923D870}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F727794-D41E-4DC0-970F-ABBB1A3142A1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="1" xr2:uid="{F54C853C-15F0-477F-87CB-91BEF9AD06FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2310" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="487">
   <si>
     <t>Basic JavaScript</t>
   </si>
@@ -1439,6 +1439,66 @@
   </si>
   <si>
     <t>PassedFind the Longest Word in a String</t>
+  </si>
+  <si>
+    <t>PassedReturn Largest Numbers in Arrays</t>
+  </si>
+  <si>
+    <t>PassedConfirm the Ending</t>
+  </si>
+  <si>
+    <t>PassedRepeat a String Repeat a String</t>
+  </si>
+  <si>
+    <t>PassedTruncate a String</t>
+  </si>
+  <si>
+    <t>PassedFinders Keepers</t>
+  </si>
+  <si>
+    <t>PassedBoo who</t>
+  </si>
+  <si>
+    <t>PassedTitle Case a Sentence</t>
+  </si>
+  <si>
+    <t>PassedSlice and Splice</t>
+  </si>
+  <si>
+    <t>PassedFalsy Bouncer</t>
+  </si>
+  <si>
+    <t>PassedWhere do I Belong</t>
+  </si>
+  <si>
+    <t>PassedMutations</t>
+  </si>
+  <si>
+    <t>PassedChunky Monkey</t>
+  </si>
+  <si>
+    <t>PassedCreate a Basic JavaScript Object</t>
+  </si>
+  <si>
+    <t>PassedUse Dot Notation to Access the Properties of an Object</t>
+  </si>
+  <si>
+    <t>PassedCreate a Method on an Object</t>
+  </si>
+  <si>
+    <t>PassedMake Code More Reusable with the this Keyword</t>
+  </si>
+  <si>
+    <t>PassedDefine a Constructor Function</t>
+  </si>
+  <si>
+    <t>PassedUse a Constructor to Create Objects</t>
+  </si>
+  <si>
+    <t>PassedExtend Constructors to Receive Arguments</t>
+  </si>
+  <si>
+    <t>PassedVerify an Object's Constructor with instanceof</t>
   </si>
 </sst>
 </file>
@@ -7958,10 +8018,10 @@
   <dimension ref="A1:H302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B208" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B220" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E209" sqref="E209"/>
+      <selection pane="bottomRight" activeCell="E230" sqref="E230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -11652,8 +11712,8 @@
       <c r="E204" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="F204" s="12">
-        <v>43469</v>
+      <c r="F204" s="2">
+        <v>43525</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.75">
@@ -11669,8 +11729,8 @@
       <c r="E205" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="F205" s="12">
-        <v>43469</v>
+      <c r="F205" s="2">
+        <v>43525</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.75">
@@ -11687,7 +11747,7 @@
         <v>464</v>
       </c>
       <c r="F206" s="2">
-        <v>43470</v>
+        <v>43525</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.75">
@@ -11704,7 +11764,7 @@
         <v>465</v>
       </c>
       <c r="F207" s="2">
-        <v>43470</v>
+        <v>43525</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.75">
@@ -11721,7 +11781,7 @@
         <v>466</v>
       </c>
       <c r="F208" s="2">
-        <v>43470</v>
+        <v>43525</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.75">
@@ -11734,11 +11794,11 @@
       <c r="C209" s="1">
         <v>208</v>
       </c>
-      <c r="E209" s="13" t="s">
-        <v>215</v>
+      <c r="E209" s="8" t="s">
+        <v>467</v>
       </c>
       <c r="F209" s="2">
-        <v>43470</v>
+        <v>43525</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.75">
@@ -11751,11 +11811,11 @@
       <c r="C210" s="1">
         <v>209</v>
       </c>
-      <c r="E210" s="13" t="s">
-        <v>216</v>
+      <c r="E210" s="8" t="s">
+        <v>468</v>
       </c>
       <c r="F210" s="2">
-        <v>43470</v>
+        <v>43525</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.75">
@@ -11768,11 +11828,11 @@
       <c r="C211" s="1">
         <v>210</v>
       </c>
-      <c r="E211" s="13" t="s">
-        <v>217</v>
+      <c r="E211" s="8" t="s">
+        <v>469</v>
       </c>
       <c r="F211" s="2">
-        <v>43470</v>
+        <v>43525</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.75">
@@ -11785,11 +11845,11 @@
       <c r="C212" s="1">
         <v>211</v>
       </c>
-      <c r="E212" s="13" t="s">
-        <v>218</v>
+      <c r="E212" s="8" t="s">
+        <v>470</v>
       </c>
       <c r="F212" s="2">
-        <v>43470</v>
+        <v>43525</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.75">
@@ -11802,11 +11862,11 @@
       <c r="C213" s="1">
         <v>212</v>
       </c>
-      <c r="E213" s="13" t="s">
-        <v>219</v>
+      <c r="E213" s="8" t="s">
+        <v>471</v>
       </c>
       <c r="F213" s="2">
-        <v>43470</v>
+        <v>43525</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.75">
@@ -11819,11 +11879,11 @@
       <c r="C214" s="1">
         <v>213</v>
       </c>
-      <c r="E214" s="13" t="s">
-        <v>220</v>
+      <c r="E214" s="8" t="s">
+        <v>472</v>
       </c>
       <c r="F214" s="2">
-        <v>43470</v>
+        <v>43525</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.75">
@@ -11836,11 +11896,11 @@
       <c r="C215" s="1">
         <v>214</v>
       </c>
-      <c r="E215" s="13" t="s">
-        <v>221</v>
+      <c r="E215" s="8" t="s">
+        <v>473</v>
       </c>
       <c r="F215" s="2">
-        <v>43470</v>
+        <v>43525</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.75">
@@ -11853,11 +11913,11 @@
       <c r="C216" s="1">
         <v>215</v>
       </c>
-      <c r="E216" s="13" t="s">
-        <v>222</v>
+      <c r="E216" s="8" t="s">
+        <v>474</v>
       </c>
       <c r="F216" s="2">
-        <v>43471</v>
+        <v>43525</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.75">
@@ -11870,11 +11930,11 @@
       <c r="C217" s="1">
         <v>216</v>
       </c>
-      <c r="E217" s="13" t="s">
-        <v>223</v>
+      <c r="E217" s="8" t="s">
+        <v>475</v>
       </c>
       <c r="F217" s="2">
-        <v>43471</v>
+        <v>43526</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.75">
@@ -11887,11 +11947,11 @@
       <c r="C218" s="1">
         <v>217</v>
       </c>
-      <c r="E218" s="13" t="s">
-        <v>224</v>
+      <c r="E218" s="8" t="s">
+        <v>476</v>
       </c>
       <c r="F218" s="2">
-        <v>43471</v>
+        <v>43526</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.75">
@@ -11904,11 +11964,11 @@
       <c r="C219" s="1">
         <v>218</v>
       </c>
-      <c r="E219" s="13" t="s">
-        <v>225</v>
+      <c r="E219" s="8" t="s">
+        <v>477</v>
       </c>
       <c r="F219" s="2">
-        <v>43471</v>
+        <v>43526</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.75">
@@ -11921,11 +11981,11 @@
       <c r="C220" s="1">
         <v>219</v>
       </c>
-      <c r="E220" s="13" t="s">
-        <v>226</v>
+      <c r="E220" s="8" t="s">
+        <v>478</v>
       </c>
       <c r="F220" s="2">
-        <v>43471</v>
+        <v>43526</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.75">
@@ -11938,11 +11998,11 @@
       <c r="C221" s="1">
         <v>220</v>
       </c>
-      <c r="E221" s="13" t="s">
+      <c r="E221" s="8" t="s">
         <v>228</v>
       </c>
       <c r="F221" s="2">
-        <v>43471</v>
+        <v>43526</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.75">
@@ -11955,11 +12015,11 @@
       <c r="C222" s="1">
         <v>221</v>
       </c>
-      <c r="E222" s="13" t="s">
-        <v>229</v>
+      <c r="E222" s="8" t="s">
+        <v>479</v>
       </c>
       <c r="F222" s="2">
-        <v>43471</v>
+        <v>43526</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.75">
@@ -11972,11 +12032,11 @@
       <c r="C223" s="1">
         <v>222</v>
       </c>
-      <c r="E223" s="13" t="s">
-        <v>230</v>
+      <c r="E223" s="8" t="s">
+        <v>480</v>
       </c>
       <c r="F223" s="2">
-        <v>43471</v>
+        <v>43526</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.75">
@@ -11989,11 +12049,11 @@
       <c r="C224" s="1">
         <v>223</v>
       </c>
-      <c r="E224" s="13" t="s">
-        <v>231</v>
+      <c r="E224" s="8" t="s">
+        <v>481</v>
       </c>
       <c r="F224" s="2">
-        <v>43471</v>
+        <v>43526</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.75">
@@ -12006,11 +12066,11 @@
       <c r="C225" s="1">
         <v>224</v>
       </c>
-      <c r="E225" s="13" t="s">
-        <v>232</v>
+      <c r="E225" s="8" t="s">
+        <v>482</v>
       </c>
       <c r="F225" s="2">
-        <v>43471</v>
+        <v>43526</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.75">
@@ -12023,11 +12083,11 @@
       <c r="C226" s="1">
         <v>225</v>
       </c>
-      <c r="E226" s="13" t="s">
-        <v>233</v>
+      <c r="E226" s="8" t="s">
+        <v>483</v>
       </c>
       <c r="F226" s="2">
-        <v>43472</v>
+        <v>43526</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.75">
@@ -12040,11 +12100,11 @@
       <c r="C227" s="1">
         <v>226</v>
       </c>
-      <c r="E227" s="13" t="s">
-        <v>234</v>
+      <c r="E227" s="8" t="s">
+        <v>484</v>
       </c>
       <c r="F227" s="2">
-        <v>43472</v>
+        <v>43527</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.75">
@@ -12057,11 +12117,11 @@
       <c r="C228" s="1">
         <v>227</v>
       </c>
-      <c r="E228" s="13" t="s">
-        <v>235</v>
+      <c r="E228" s="8" t="s">
+        <v>485</v>
       </c>
       <c r="F228" s="2">
-        <v>43472</v>
+        <v>43527</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.75">
@@ -12074,11 +12134,11 @@
       <c r="C229" s="1">
         <v>228</v>
       </c>
-      <c r="E229" s="13" t="s">
-        <v>236</v>
+      <c r="E229" s="8" t="s">
+        <v>486</v>
       </c>
       <c r="F229" s="2">
-        <v>43472</v>
+        <v>43527</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.75">
@@ -12095,7 +12155,7 @@
         <v>237</v>
       </c>
       <c r="F230" s="2">
-        <v>43472</v>
+        <v>43527</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.75">
@@ -12112,7 +12172,7 @@
         <v>238</v>
       </c>
       <c r="F231" s="2">
-        <v>43472</v>
+        <v>43527</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.75">
@@ -12129,7 +12189,7 @@
         <v>239</v>
       </c>
       <c r="F232" s="2">
-        <v>43472</v>
+        <v>43527</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.75">
@@ -12146,7 +12206,7 @@
         <v>240</v>
       </c>
       <c r="F233" s="2">
-        <v>43472</v>
+        <v>43527</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.75">
@@ -12163,7 +12223,7 @@
         <v>241</v>
       </c>
       <c r="F234" s="2">
-        <v>43472</v>
+        <v>43527</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.75">
@@ -12180,7 +12240,7 @@
         <v>242</v>
       </c>
       <c r="F235" s="2">
-        <v>43472</v>
+        <v>43527</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.75">
@@ -12197,7 +12257,7 @@
         <v>243</v>
       </c>
       <c r="F236" s="2">
-        <v>43473</v>
+        <v>43527</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.75">
@@ -12214,7 +12274,7 @@
         <v>244</v>
       </c>
       <c r="F237" s="2">
-        <v>43473</v>
+        <v>43528</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.75">
@@ -12231,7 +12291,7 @@
         <v>245</v>
       </c>
       <c r="F238" s="2">
-        <v>43473</v>
+        <v>43528</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.75">
@@ -12248,7 +12308,7 @@
         <v>246</v>
       </c>
       <c r="F239" s="2">
-        <v>43473</v>
+        <v>43528</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.75">
@@ -12265,7 +12325,7 @@
         <v>247</v>
       </c>
       <c r="F240" s="2">
-        <v>43473</v>
+        <v>43528</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.75">
@@ -12282,7 +12342,7 @@
         <v>248</v>
       </c>
       <c r="F241" s="2">
-        <v>43473</v>
+        <v>43528</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.75">
@@ -12299,7 +12359,7 @@
         <v>249</v>
       </c>
       <c r="F242" s="2">
-        <v>43473</v>
+        <v>43528</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.75">
@@ -12316,7 +12376,7 @@
         <v>250</v>
       </c>
       <c r="F243" s="2">
-        <v>43473</v>
+        <v>43528</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.75">
@@ -12333,7 +12393,7 @@
         <v>251</v>
       </c>
       <c r="F244" s="2">
-        <v>43473</v>
+        <v>43528</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.75">
@@ -12350,7 +12410,7 @@
         <v>252</v>
       </c>
       <c r="F245" s="2">
-        <v>43473</v>
+        <v>43528</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.75">
@@ -12367,7 +12427,7 @@
         <v>253</v>
       </c>
       <c r="F246" s="2">
-        <v>43474</v>
+        <v>43528</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.75">
@@ -12384,7 +12444,7 @@
         <v>254</v>
       </c>
       <c r="F247" s="2">
-        <v>43474</v>
+        <v>43529</v>
       </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.75">
@@ -12401,7 +12461,7 @@
         <v>256</v>
       </c>
       <c r="F248" s="2">
-        <v>43474</v>
+        <v>43529</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.75">
@@ -12418,7 +12478,7 @@
         <v>257</v>
       </c>
       <c r="F249" s="2">
-        <v>43474</v>
+        <v>43529</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.75">
@@ -12435,7 +12495,7 @@
         <v>258</v>
       </c>
       <c r="F250" s="2">
-        <v>43474</v>
+        <v>43529</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.75">
@@ -12452,7 +12512,7 @@
         <v>259</v>
       </c>
       <c r="F251" s="2">
-        <v>43474</v>
+        <v>43529</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.75">
@@ -12469,7 +12529,7 @@
         <v>260</v>
       </c>
       <c r="F252" s="2">
-        <v>43474</v>
+        <v>43529</v>
       </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.75">
@@ -12486,7 +12546,7 @@
         <v>261</v>
       </c>
       <c r="F253" s="2">
-        <v>43474</v>
+        <v>43529</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.75">
@@ -12503,7 +12563,7 @@
         <v>262</v>
       </c>
       <c r="F254" s="2">
-        <v>43474</v>
+        <v>43529</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.75">
@@ -12520,7 +12580,7 @@
         <v>263</v>
       </c>
       <c r="F255" s="2">
-        <v>43474</v>
+        <v>43529</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.75">
@@ -12537,7 +12597,7 @@
         <v>264</v>
       </c>
       <c r="F256" s="2">
-        <v>43475</v>
+        <v>43529</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.75">
@@ -12554,7 +12614,7 @@
         <v>265</v>
       </c>
       <c r="F257" s="2">
-        <v>43475</v>
+        <v>43530</v>
       </c>
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.75">
@@ -12571,7 +12631,7 @@
         <v>266</v>
       </c>
       <c r="F258" s="2">
-        <v>43475</v>
+        <v>43530</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.75">
@@ -12588,7 +12648,7 @@
         <v>267</v>
       </c>
       <c r="F259" s="2">
-        <v>43475</v>
+        <v>43530</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.75">
@@ -12605,7 +12665,7 @@
         <v>268</v>
       </c>
       <c r="F260" s="2">
-        <v>43475</v>
+        <v>43530</v>
       </c>
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.75">
@@ -12622,7 +12682,7 @@
         <v>269</v>
       </c>
       <c r="F261" s="2">
-        <v>43475</v>
+        <v>43530</v>
       </c>
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.75">
@@ -12639,7 +12699,7 @@
         <v>270</v>
       </c>
       <c r="F262" s="2">
-        <v>43475</v>
+        <v>43530</v>
       </c>
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.75">
@@ -12656,7 +12716,7 @@
         <v>271</v>
       </c>
       <c r="F263" s="2">
-        <v>43475</v>
+        <v>43530</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.75">
@@ -12673,7 +12733,7 @@
         <v>272</v>
       </c>
       <c r="F264" s="2">
-        <v>43475</v>
+        <v>43530</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.75">
@@ -12690,7 +12750,7 @@
         <v>273</v>
       </c>
       <c r="F265" s="2">
-        <v>43475</v>
+        <v>43530</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.75">
@@ -12707,7 +12767,7 @@
         <v>274</v>
       </c>
       <c r="F266" s="2">
-        <v>43476</v>
+        <v>43530</v>
       </c>
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.75">
@@ -12724,7 +12784,7 @@
         <v>275</v>
       </c>
       <c r="F267" s="2">
-        <v>43476</v>
+        <v>43531</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.75">
@@ -12741,7 +12801,7 @@
         <v>276</v>
       </c>
       <c r="F268" s="2">
-        <v>43476</v>
+        <v>43531</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.75">
@@ -12758,7 +12818,7 @@
         <v>277</v>
       </c>
       <c r="F269" s="2">
-        <v>43476</v>
+        <v>43531</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.75">
@@ -12775,7 +12835,7 @@
         <v>278</v>
       </c>
       <c r="F270" s="2">
-        <v>43476</v>
+        <v>43531</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.75">
@@ -12792,7 +12852,7 @@
         <v>279</v>
       </c>
       <c r="F271" s="2">
-        <v>43476</v>
+        <v>43531</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.75">
@@ -12809,7 +12869,7 @@
         <v>281</v>
       </c>
       <c r="F272" s="2">
-        <v>43476</v>
+        <v>43531</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.75">
@@ -12826,7 +12886,7 @@
         <v>282</v>
       </c>
       <c r="F273" s="2">
-        <v>43476</v>
+        <v>43531</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.75">
@@ -12843,7 +12903,7 @@
         <v>283</v>
       </c>
       <c r="F274" s="2">
-        <v>43476</v>
+        <v>43531</v>
       </c>
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.75">
@@ -12860,7 +12920,7 @@
         <v>284</v>
       </c>
       <c r="F275" s="2">
-        <v>43476</v>
+        <v>43531</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.75">
@@ -12877,7 +12937,7 @@
         <v>285</v>
       </c>
       <c r="F276" s="2">
-        <v>43477</v>
+        <v>43531</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.75">
@@ -12894,7 +12954,7 @@
         <v>286</v>
       </c>
       <c r="F277" s="2">
-        <v>43477</v>
+        <v>43532</v>
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.75">
@@ -12911,7 +12971,7 @@
         <v>287</v>
       </c>
       <c r="F278" s="2">
-        <v>43477</v>
+        <v>43532</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.75">
@@ -12928,7 +12988,7 @@
         <v>288</v>
       </c>
       <c r="F279" s="2">
-        <v>43477</v>
+        <v>43532</v>
       </c>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.75">
@@ -12945,7 +13005,7 @@
         <v>289</v>
       </c>
       <c r="F280" s="2">
-        <v>43477</v>
+        <v>43532</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.75">
@@ -12962,7 +13022,7 @@
         <v>290</v>
       </c>
       <c r="F281" s="2">
-        <v>43477</v>
+        <v>43532</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.75">
@@ -12979,7 +13039,7 @@
         <v>291</v>
       </c>
       <c r="F282" s="2">
-        <v>43477</v>
+        <v>43532</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.75">
@@ -12996,7 +13056,7 @@
         <v>292</v>
       </c>
       <c r="F283" s="2">
-        <v>43477</v>
+        <v>43532</v>
       </c>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.75">
@@ -13013,7 +13073,7 @@
         <v>293</v>
       </c>
       <c r="F284" s="2">
-        <v>43477</v>
+        <v>43532</v>
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.75">
@@ -13030,7 +13090,7 @@
         <v>294</v>
       </c>
       <c r="F285" s="2">
-        <v>43477</v>
+        <v>43532</v>
       </c>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.75">
@@ -13047,7 +13107,7 @@
         <v>295</v>
       </c>
       <c r="F286" s="2">
-        <v>43478</v>
+        <v>43532</v>
       </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.75">
@@ -13064,7 +13124,7 @@
         <v>296</v>
       </c>
       <c r="F287" s="2">
-        <v>43478</v>
+        <v>43533</v>
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.75">
@@ -13081,7 +13141,7 @@
         <v>297</v>
       </c>
       <c r="F288" s="2">
-        <v>43478</v>
+        <v>43533</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.75">
@@ -13098,7 +13158,7 @@
         <v>298</v>
       </c>
       <c r="F289" s="2">
-        <v>43478</v>
+        <v>43533</v>
       </c>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.75">
@@ -13115,7 +13175,7 @@
         <v>299</v>
       </c>
       <c r="F290" s="2">
-        <v>43478</v>
+        <v>43533</v>
       </c>
     </row>
     <row r="291" spans="1:6" x14ac:dyDescent="0.75">
@@ -13132,7 +13192,7 @@
         <v>300</v>
       </c>
       <c r="F291" s="2">
-        <v>43478</v>
+        <v>43533</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.75">
@@ -13149,7 +13209,7 @@
         <v>301</v>
       </c>
       <c r="F292" s="2">
-        <v>43478</v>
+        <v>43533</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.75">
@@ -13166,7 +13226,7 @@
         <v>302</v>
       </c>
       <c r="F293" s="2">
-        <v>43478</v>
+        <v>43533</v>
       </c>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.75">
@@ -13183,7 +13243,7 @@
         <v>304</v>
       </c>
       <c r="F294" s="2">
-        <v>43478</v>
+        <v>43533</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.75">
@@ -13200,7 +13260,7 @@
         <v>305</v>
       </c>
       <c r="F295" s="2">
-        <v>43478</v>
+        <v>43533</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.75">
@@ -13217,7 +13277,7 @@
         <v>306</v>
       </c>
       <c r="F296" s="2">
-        <v>43479</v>
+        <v>43533</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.75">
@@ -13234,7 +13294,7 @@
         <v>307</v>
       </c>
       <c r="F297" s="2">
-        <v>43479</v>
+        <v>43534</v>
       </c>
     </row>
     <row r="298" spans="1:6" x14ac:dyDescent="0.75">
@@ -13251,7 +13311,7 @@
         <v>308</v>
       </c>
       <c r="F298" s="2">
-        <v>43479</v>
+        <v>43534</v>
       </c>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.75">
@@ -13268,7 +13328,7 @@
         <v>309</v>
       </c>
       <c r="F299" s="2">
-        <v>43479</v>
+        <v>43534</v>
       </c>
     </row>
     <row r="301" spans="1:6" x14ac:dyDescent="0.75">

</xml_diff>